<commit_message>
Escaldar por pistola de agua
</commit_message>
<xml_diff>
--- a/Movimientos.xlsx
+++ b/Movimientos.xlsx
@@ -1,10 +1,1586 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\user\pokecrystal-newbox\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17895" windowHeight="8145"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
+</workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="292">
+  <si>
+    <t>ACERO</t>
+  </si>
+  <si>
+    <t>AGUA</t>
+  </si>
+  <si>
+    <t>BICHO</t>
+  </si>
+  <si>
+    <t>DRAGÓN</t>
+  </si>
+  <si>
+    <t>ELÉCTRICO</t>
+  </si>
+  <si>
+    <t>FANTASMA</t>
+  </si>
+  <si>
+    <t>FUEGO</t>
+  </si>
+  <si>
+    <t>HADA</t>
+  </si>
+  <si>
+    <t>HIELO</t>
+  </si>
+  <si>
+    <t>LUCHA</t>
+  </si>
+  <si>
+    <t>NORMAL</t>
+  </si>
+  <si>
+    <t>PLANTA</t>
+  </si>
+  <si>
+    <t>ROCA</t>
+  </si>
+  <si>
+    <t>PSÍQUICO</t>
+  </si>
+  <si>
+    <t>SINIESTRO</t>
+  </si>
+  <si>
+    <t>TIERRA</t>
+  </si>
+  <si>
+    <t>VENENO</t>
+  </si>
+  <si>
+    <t>VOLADOR</t>
+  </si>
+  <si>
+    <t>Físico</t>
+  </si>
+  <si>
+    <t>Especial</t>
+  </si>
+  <si>
+    <t>Doblebofetón (15x2a5) - 85</t>
+  </si>
+  <si>
+    <t>Destructor (40) - 100</t>
+  </si>
+  <si>
+    <t>Puño cometa (18x2a5) - 85</t>
+  </si>
+  <si>
+    <t>Golpe Kárate (50) - 100</t>
+  </si>
+  <si>
+    <t>Día de pago (40) - 100</t>
+  </si>
+  <si>
+    <t>Puño fuego (75) - 100</t>
+  </si>
+  <si>
+    <t>Puño hielo (75) - 100</t>
+  </si>
+  <si>
+    <t>Puño trueno (75) - 100</t>
+  </si>
+  <si>
+    <t>Arañazo (40) - 100</t>
+  </si>
+  <si>
+    <t>Placaje (40) - 100</t>
+  </si>
+  <si>
+    <t>Tenaza (55) - 100</t>
+  </si>
+  <si>
+    <t>ONE HIT KO</t>
+  </si>
+  <si>
+    <t>Guillotina</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Viento cortante (80) - 100</t>
+  </si>
+  <si>
+    <t>POTENCIADORES</t>
+  </si>
+  <si>
+    <t>Ataque</t>
+  </si>
+  <si>
+    <t>Defensa</t>
+  </si>
+  <si>
+    <t>Velocidad</t>
+  </si>
+  <si>
+    <t>At. Especial</t>
+  </si>
+  <si>
+    <t>Defensa Especial</t>
+  </si>
+  <si>
+    <t>Danza espada (2 niveles)</t>
+  </si>
+  <si>
+    <t>Tornado (40) - 100</t>
+  </si>
+  <si>
+    <t>Ataque ala (60) - 100</t>
+  </si>
+  <si>
+    <t>Remolino</t>
+  </si>
+  <si>
+    <t>IMPIDE POKEMON HUYA</t>
+  </si>
+  <si>
+    <t>Atadura</t>
+  </si>
+  <si>
+    <t>2 a 5 turnos</t>
+  </si>
+  <si>
+    <t>Atizar (80) -75</t>
+  </si>
+  <si>
+    <t>Látigo cepa (45) - 100</t>
+  </si>
+  <si>
+    <t>Pisotón (65) -100</t>
+  </si>
+  <si>
+    <t>Doble patada (30x2) - 100</t>
+  </si>
+  <si>
+    <t>Megapatada (120) -75</t>
+  </si>
+  <si>
+    <t>Patada salto (100) - 95</t>
+  </si>
+  <si>
+    <t>DEBILITADORES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precisión </t>
+  </si>
+  <si>
+    <t>Patada giro (60) - 85</t>
+  </si>
+  <si>
+    <t>Ataque arena (1 nivel) - 100</t>
+  </si>
+  <si>
+    <t>Golpe cabeza (70) - 100</t>
+  </si>
+  <si>
+    <t>Cornada (65) -100</t>
+  </si>
+  <si>
+    <t>Ataque furia (15x2a5) - 85</t>
+  </si>
+  <si>
+    <t>Perforador</t>
+  </si>
+  <si>
+    <t>Golpe cuerpo (85) - 100</t>
+  </si>
+  <si>
+    <t>Constricción (15x2a5) - 90</t>
+  </si>
+  <si>
+    <t>Derribo (90) - 85</t>
+  </si>
+  <si>
+    <t>Golpe (120) - 100</t>
+  </si>
+  <si>
+    <t>Doble filo (120) - 100</t>
+  </si>
+  <si>
+    <t>Látigo (1 nivel) - 100</t>
+  </si>
+  <si>
+    <t>Picotazo ven (15) - 100</t>
+  </si>
+  <si>
+    <t>Doble ataque (25x2) - 100</t>
+  </si>
+  <si>
+    <t>Pin Misil (25x2a5) - 95</t>
+  </si>
+  <si>
+    <t>Malicioso (1 nivel) - 100</t>
+  </si>
+  <si>
+    <t>Mordisco (60) - 100</t>
+  </si>
+  <si>
+    <t>Gruñido (1 nivel) - 100</t>
+  </si>
+  <si>
+    <t>Rugido</t>
+  </si>
+  <si>
+    <t>(18) - 85</t>
+  </si>
+  <si>
+    <t>Bomba sónica (20 ps)</t>
+  </si>
+  <si>
+    <t>Ácido (40) - 100)</t>
+  </si>
+  <si>
+    <t>Ascuas (40) -100</t>
+  </si>
+  <si>
+    <t>Lanzallamas (95) - 100</t>
+  </si>
+  <si>
+    <t>Pistola agua (40) -100</t>
+  </si>
+  <si>
+    <t>Hidrobomba (120) - 80</t>
+  </si>
+  <si>
+    <t>Surf (95) - 100</t>
+  </si>
+  <si>
+    <t>Rayo hielo (95) - 100</t>
+  </si>
+  <si>
+    <t>Ventisca (120) - 70</t>
+  </si>
+  <si>
+    <t>Psicorrayo (65) - 100</t>
+  </si>
+  <si>
+    <t>Rayo burbuja (65) - 100</t>
+  </si>
+  <si>
+    <t>Rayo aurora (65) - 100</t>
+  </si>
+  <si>
+    <t>Hiperrayo (150) - 90</t>
+  </si>
+  <si>
+    <t>Picotazo (35)</t>
+  </si>
+  <si>
+    <t>Pico taladro (80) - 100</t>
+  </si>
+  <si>
+    <t>Sumisión (80) -80</t>
+  </si>
+  <si>
+    <t>Patada baja (50) - 100</t>
+  </si>
+  <si>
+    <t>Golpe sísmico (-) - 100</t>
+  </si>
+  <si>
+    <t>Fuerza (80) - 100</t>
+  </si>
+  <si>
+    <t>Absorber (20) - 100</t>
+  </si>
+  <si>
+    <t>Desarrollo (1 nivel)</t>
+  </si>
+  <si>
+    <t>Hoja afilada (55) - 95</t>
+  </si>
+  <si>
+    <t>Rayo solar (120) - 100</t>
+  </si>
+  <si>
+    <t>Megaagotar (40) -100</t>
+  </si>
+  <si>
+    <t>ALTERACIONES DE ESTADO</t>
+  </si>
+  <si>
+    <t>Dormir</t>
+  </si>
+  <si>
+    <t>Canto (55)</t>
+  </si>
+  <si>
+    <t>Veneno</t>
+  </si>
+  <si>
+    <t>Polvo veneno (75)</t>
+  </si>
+  <si>
+    <t>Paralizar</t>
+  </si>
+  <si>
+    <t>Paralizador (75)</t>
+  </si>
+  <si>
+    <t>Somnífero (75)</t>
+  </si>
+  <si>
+    <t>Danza pétalo (120) - 100</t>
+  </si>
+  <si>
+    <t>Disparo demora (1 nivel) - 95</t>
+  </si>
+  <si>
+    <t>Furia dragón (40 ps)</t>
+  </si>
+  <si>
+    <t>Giro fuego (35x2a5) -85</t>
+  </si>
+  <si>
+    <t>Impactrueno (40) -100</t>
+  </si>
+  <si>
+    <t>Rayo (95) - 100</t>
+  </si>
+  <si>
+    <t>Onda trueno (100)</t>
+  </si>
+  <si>
+    <t>Lanzarrocas (50) -90</t>
+  </si>
+  <si>
+    <t>Terremoto (100) -100</t>
+  </si>
+  <si>
+    <t>Fisura</t>
+  </si>
+  <si>
+    <t>Tierra</t>
+  </si>
+  <si>
+    <t>30% + diff nivel</t>
+  </si>
+  <si>
+    <t>Necesita tener más nivel que el enemigo</t>
+  </si>
+  <si>
+    <t>Necesita tener más velocidad que el enemigo</t>
+  </si>
+  <si>
+    <t>Excavar (80) - 100</t>
+  </si>
+  <si>
+    <t>Tóxico (90)</t>
+  </si>
+  <si>
+    <t>Confusión (50) - 100</t>
+  </si>
+  <si>
+    <t>Psíquico (90) - 100</t>
+  </si>
+  <si>
+    <t>Hipnosis (60)</t>
+  </si>
+  <si>
+    <t>Meditación (1 nivel)</t>
+  </si>
+  <si>
+    <t>Agilidad (2 niveles)</t>
+  </si>
+  <si>
+    <t>Ataque rapido (40) - 100</t>
+  </si>
+  <si>
+    <t>Furia (20) - 100</t>
+  </si>
+  <si>
+    <t>Tinieblas (-) - 100</t>
+  </si>
+  <si>
+    <t>Evasión</t>
+  </si>
+  <si>
+    <t>Recuperación</t>
+  </si>
+  <si>
+    <t>Viento plata (60) - 100</t>
+  </si>
+  <si>
+    <t>Reducción (1 nivel)</t>
+  </si>
+  <si>
+    <t>Chirrido (2 niveles) - 100</t>
+  </si>
+  <si>
+    <t>Pantalla humo (1 nivel) 100</t>
+  </si>
+  <si>
+    <t>Destello (1 nivel) - 100</t>
+  </si>
+  <si>
+    <t>Refugio (1 nivel)</t>
+  </si>
+  <si>
+    <t>Rizo defensa (1 nivel)</t>
+  </si>
+  <si>
+    <t>Barrera (2 niveles)</t>
+  </si>
+  <si>
+    <t>*Pantalla luz (5 turnos)</t>
+  </si>
+  <si>
+    <t>Neblina</t>
+  </si>
+  <si>
+    <t>Niebla</t>
+  </si>
+  <si>
+    <t>Restablece los cambios de carácterísticas de todos los Pokemon</t>
+  </si>
+  <si>
+    <t>*Reflejo (5 turnos)</t>
+  </si>
+  <si>
+    <t>Autodestrucción (200) - 100</t>
+  </si>
+  <si>
+    <t>Bomba huevo (100) - 75</t>
+  </si>
+  <si>
+    <t>Lengüetazo (30) -100</t>
+  </si>
+  <si>
+    <t>Polución (30) - 70</t>
+  </si>
+  <si>
+    <t>Residuos (65) - 100</t>
+  </si>
+  <si>
+    <t>Hueso palo (65) - 85</t>
+  </si>
+  <si>
+    <t>Llamarada (120) -85</t>
+  </si>
+  <si>
+    <t>Cascada (80) - 100</t>
+  </si>
+  <si>
+    <t>Tenaza (35x2a5) - 85</t>
+  </si>
+  <si>
+    <t>Rapidez (60) - 100</t>
+  </si>
+  <si>
+    <t>Cabezazo (130) -100</t>
+  </si>
+  <si>
+    <t>Clavo cañón (20x2a5) -100</t>
+  </si>
+  <si>
+    <t>Restricción (10) - 100</t>
+  </si>
+  <si>
+    <t>Amnesia (2 niveles)</t>
+  </si>
+  <si>
+    <t>Kinético (1 nivel) - 80</t>
+  </si>
+  <si>
+    <t>Amortiguador</t>
+  </si>
+  <si>
+    <t>Patada Alta (130) - 90</t>
+  </si>
+  <si>
+    <t>Deslumbrar (100)</t>
+  </si>
+  <si>
+    <t>Comesueños (100) - 100</t>
+  </si>
+  <si>
+    <t>Gas venenoso (90)</t>
+  </si>
+  <si>
+    <t>Bombardeo (15x2a5) - 85</t>
+  </si>
+  <si>
+    <t>Chupavidas (80) - 100</t>
+  </si>
+  <si>
+    <t>Ataque aéreo (140) - 90</t>
+  </si>
+  <si>
+    <t>Beso amoroso (75)</t>
+  </si>
+  <si>
+    <t>Burbuja (40) - 100</t>
+  </si>
+  <si>
+    <t>Puño mareo (70) - 100</t>
+  </si>
+  <si>
+    <t>Espora (100)</t>
+  </si>
+  <si>
+    <t>Psicoonda (-) - 100</t>
+  </si>
+  <si>
+    <t>Armadura ácida (2 niveles)</t>
+  </si>
+  <si>
+    <t>Martillazo (100) - 90</t>
+  </si>
+  <si>
+    <t>Explosión (250) - 100</t>
+  </si>
+  <si>
+    <t>Golpes furia (18x2a5) - 85</t>
+  </si>
+  <si>
+    <t>Avalancha (75) - 90</t>
+  </si>
+  <si>
+    <t>Hipercolmillo (80) - 90</t>
+  </si>
+  <si>
+    <t>Afilar (1 nivel)</t>
+  </si>
+  <si>
+    <t>Tri ataque (80) - 100</t>
+  </si>
+  <si>
+    <t>Superdiente (mitad PS actuales)</t>
+  </si>
+  <si>
+    <t>Cuchillada (70) - 100</t>
+  </si>
+  <si>
+    <t>Triple patada (10+20+30) - 100</t>
+  </si>
+  <si>
+    <t>Ladrón (60) -100</t>
+  </si>
+  <si>
+    <t>Telaraña</t>
+  </si>
+  <si>
+    <t>Pesadilla (1/4 max PS) -100</t>
+  </si>
+  <si>
+    <t>Rueda fuego (60) - 100</t>
+  </si>
+  <si>
+    <t>Ronquido (50) -  100</t>
+  </si>
+  <si>
+    <t>Aerochorro (100) - 95</t>
+  </si>
+  <si>
+    <t>Esporadogón (2 niveles) - 100</t>
+  </si>
+  <si>
+    <t>Nieve polvo (40) -100)</t>
+  </si>
+  <si>
+    <t>Ultrapuño (40) - 100</t>
+  </si>
+  <si>
+    <t>Cara susto (2 niveles) - 100</t>
+  </si>
+  <si>
+    <t>Finta (60) - 100</t>
+  </si>
+  <si>
+    <t>Bomba lodo (90) - 100</t>
+  </si>
+  <si>
+    <t>Bofetón lodo (20) - 100</t>
+  </si>
+  <si>
+    <t>Pulpocañón (65) - 85</t>
+  </si>
+  <si>
+    <t>Electrocañón (120) -50</t>
+  </si>
+  <si>
+    <t>Viento hielo (55) - 95</t>
+  </si>
+  <si>
+    <t>Ataque óseo (25x2a5) - 90</t>
+  </si>
+  <si>
+    <t>Enfado (120) -100</t>
+  </si>
+  <si>
+    <t>Gigadrenado (75) - 100</t>
+  </si>
+  <si>
+    <t>Encanto (2 niveles)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batido </t>
+  </si>
+  <si>
+    <t>Chispa (65) - 100</t>
+  </si>
+  <si>
+    <t>Corte furia (40) - 95</t>
+  </si>
+  <si>
+    <t>Ala de acero (70) - 90</t>
+  </si>
+  <si>
+    <t>Mal de ojo</t>
+  </si>
+  <si>
+    <t>Fuegosagrado (100) -95</t>
+  </si>
+  <si>
+    <t>Magnitud (variable)</t>
+  </si>
+  <si>
+    <t>Puño dinámico (100) - 50</t>
+  </si>
+  <si>
+    <t>Megacuerno (120) - 85</t>
+  </si>
+  <si>
+    <t>Dragoaliento (60) - 100</t>
+  </si>
+  <si>
+    <t>Persecución (40) - 100</t>
+  </si>
+  <si>
+    <t>Giro rápido (50) - 100</t>
+  </si>
+  <si>
+    <t>Dulce aroma (1 nivel) - 100</t>
+  </si>
+  <si>
+    <t>Cola férrea (100) - 75</t>
+  </si>
+  <si>
+    <t>Garra metal (50) - 75</t>
+  </si>
+  <si>
+    <t>Tiro vital 70 -(100)</t>
+  </si>
+  <si>
+    <t>Sol matinal</t>
+  </si>
+  <si>
+    <t>Luz lunar</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Tajo cruzado (100) - 80</t>
+  </si>
+  <si>
+    <t>Ciclón (40) - 100</t>
+  </si>
+  <si>
+    <t>Triturar (80)- 100</t>
+  </si>
+  <si>
+    <t>Velocidad extrema (80) -100</t>
+  </si>
+  <si>
+    <t>Poder pasado (60) - 100</t>
+  </si>
+  <si>
+    <t>Bola sombra (80) -100</t>
+  </si>
+  <si>
+    <t>Golpe roca (40) -100</t>
+  </si>
+  <si>
+    <t>Torbellino (35) -85</t>
+  </si>
+  <si>
+    <t>Paliza (60 variables) - 100</t>
+  </si>
+  <si>
+    <t>Fuerza lunar (95) - 100</t>
+  </si>
+  <si>
+    <t>Carantoña (90)- 90</t>
+  </si>
+  <si>
+    <t>Doble equipo (1 nivel)</t>
+  </si>
+  <si>
+    <t>Quemar</t>
+  </si>
+  <si>
+    <t>Congelar</t>
+  </si>
+  <si>
+    <t>Confusión</t>
+  </si>
+  <si>
+    <t>Supersónico (55)</t>
+  </si>
+  <si>
+    <t>Beso dulce (75)</t>
+  </si>
+  <si>
+    <t>Rayo confuso (100)</t>
+  </si>
+  <si>
+    <t>MOVIMIENTOS DE EVASIÓN</t>
+  </si>
+  <si>
+    <t>IMPIDE CAMBIOS EN ESTADÍSTICAS</t>
+  </si>
+  <si>
+    <t>RECUPERACIÓN PUNTOS DE SALUD</t>
+  </si>
+  <si>
+    <t>Cabeza hierro (80) - 100</t>
+  </si>
+  <si>
+    <t>Chuzos (85) - 90</t>
+  </si>
+  <si>
+    <t>Tajo umbrío (70) -100</t>
+  </si>
+  <si>
+    <t>Puya nociva (80) - 100</t>
+  </si>
+  <si>
+    <t>Joya de luz (80) - 100</t>
+  </si>
+  <si>
+    <t>Onda mental (100)- 100</t>
+  </si>
+  <si>
+    <t>Escaldar (80) - 100</t>
+  </si>
+  <si>
+    <t>Roca afilada (100) - 80</t>
+  </si>
+  <si>
+    <t>Hidropulso (60) - 100</t>
+  </si>
+  <si>
+    <t>Voltio cruel (90) - 100</t>
+  </si>
+  <si>
+    <t>Fuego fatuo (85)</t>
+  </si>
+  <si>
+    <t>Tijera X (80) - 100</t>
+  </si>
+  <si>
+    <t>Cabezazo zen (80) - 90</t>
+  </si>
+  <si>
+    <t>Garra umbría (70) - 100</t>
+  </si>
+  <si>
+    <t>Bomba gérmen (80) - 100</t>
+  </si>
+  <si>
+    <t>Fortaleza (1 nivel)</t>
+  </si>
+  <si>
+    <t>Esquirla helada (40) - 100</t>
+  </si>
+  <si>
+    <t>Vozarrón (90) - 100</t>
+  </si>
+  <si>
+    <t>Vendaval (120) - 70</t>
+  </si>
+  <si>
+    <t>Afilagarras (1 nivel)</t>
+  </si>
+  <si>
+    <t>Precisión</t>
+  </si>
+  <si>
+    <t>Infortunio (65) - 100</t>
+  </si>
+  <si>
+    <t>Lanzamugre (120) - 80</t>
+  </si>
+  <si>
+    <t>Onda certera (120) - 70</t>
+  </si>
+  <si>
+    <t>Foco resplandor (80) - 100</t>
+  </si>
+  <si>
+    <t>Envite ígneo (120) - 100</t>
+  </si>
+  <si>
+    <t>Paranormal (80) -100</t>
+  </si>
+  <si>
+    <t>Energibola (90) -100</t>
+  </si>
+  <si>
+    <t>Tierra viva (90) - 100</t>
+  </si>
+  <si>
+    <t>Beso drenaje (50) -100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viento feérico (40) -100 </t>
+  </si>
+  <si>
+    <t>Pulso dragón (85)- 100</t>
+  </si>
+  <si>
+    <t>Voz cautivadora (40) - 100</t>
+  </si>
+  <si>
+    <t>Brillo mágico (80) - 100</t>
+  </si>
+  <si>
+    <t>Pulso umbrío (80) - 100</t>
+  </si>
+  <si>
+    <t>Paz mental ( 1 nivel)</t>
+  </si>
+  <si>
+    <t>Paz mental (1 nivel)</t>
+  </si>
+  <si>
+    <t>Puño bala (40) - 100</t>
+  </si>
+  <si>
+    <t>Corpulencia</t>
+  </si>
+  <si>
+    <t>Zumbido (90) - 100</t>
+  </si>
+  <si>
+    <t>Alud (60) - 100</t>
+  </si>
+  <si>
+    <t>Impresionar (30) - 100</t>
+  </si>
+  <si>
+    <t>Acua cola (90) - 90</t>
+  </si>
+  <si>
+    <t>Tajo aéreo (75) - 95</t>
+  </si>
+  <si>
+    <t>Golpe aéreo (60) - 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trueno (120) - 70 </t>
+  </si>
+</sst>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="16">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="68">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
+</styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF123"/>
+  <dimension ref="A1:AF117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I93" sqref="I93"/>
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33,14 +1609,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="F1" s="52" t="s">
+      <c r="C1" s="52"/>
+      <c r="F1" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="54"/>
+      <c r="G1" s="52"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
@@ -55,15 +1631,15 @@
       <c r="G2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="52" t="s">
+      <c r="I2" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="54"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="52"/>
     </row>
     <row r="3" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="14" t="s">
@@ -127,7 +1703,7 @@
       <c r="N4" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="O4" s="44"/>
+      <c r="O4" s="42"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
@@ -181,7 +1757,7 @@
         <v>108</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="48" t="s">
+      <c r="J7" s="46" t="s">
         <v>261</v>
       </c>
       <c r="K7" s="14"/>
@@ -191,7 +1767,7 @@
       <c r="O7" s="14"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="41" t="s">
         <v>283</v>
       </c>
       <c r="C8" s="10"/>
@@ -208,11 +1784,11 @@
       <c r="O8" s="14"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B9" s="43"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="10"/>
       <c r="F9" s="9"/>
       <c r="G9" s="14"/>
-      <c r="I9" s="43" t="s">
+      <c r="I9" s="41" t="s">
         <v>265</v>
       </c>
       <c r="J9" s="14" t="s">
@@ -222,35 +1798,35 @@
       <c r="L9" s="14"/>
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
-      <c r="O9" s="43" t="s">
+      <c r="O9" s="41" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="40" t="s">
         <v>270</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="17"/>
-      <c r="I10" s="40" t="s">
+      <c r="I10" s="38" t="s">
         <v>284</v>
       </c>
-      <c r="J10" s="40" t="s">
+      <c r="J10" s="38" t="s">
         <v>284</v>
       </c>
       <c r="K10" s="15"/>
-      <c r="L10" s="40" t="s">
+      <c r="L10" s="38" t="s">
         <v>281</v>
       </c>
-      <c r="M10" s="40" t="s">
+      <c r="M10" s="38" t="s">
         <v>282</v>
       </c>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
@@ -262,10 +1838,10 @@
     <row r="11" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="F11" s="45" t="s">
+      <c r="F11" s="43" t="s">
         <v>260</v>
       </c>
-      <c r="G11" s="40" t="s">
+      <c r="G11" s="38" t="s">
         <v>273</v>
       </c>
       <c r="I11" s="20"/>
@@ -290,14 +1866,14 @@
     </row>
     <row r="14" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="F14" s="52" t="s">
+      <c r="C14" s="52"/>
+      <c r="F14" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="54"/>
+      <c r="G14" s="52"/>
     </row>
     <row r="15" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
@@ -313,15 +1889,15 @@
       <c r="G15" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="52" t="s">
+      <c r="I15" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="J15" s="53"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="53"/>
-      <c r="M15" s="53"/>
-      <c r="N15" s="53"/>
-      <c r="O15" s="54"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="55"/>
+      <c r="M15" s="55"/>
+      <c r="N15" s="55"/>
+      <c r="O15" s="52"/>
     </row>
     <row r="16" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
@@ -332,7 +1908,7 @@
       <c r="F16" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="G16" s="28" t="s">
+      <c r="G16" s="26" t="s">
         <v>229</v>
       </c>
       <c r="I16" s="21" t="s">
@@ -398,12 +1974,12 @@
       <c r="K18" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="L18" s="49"/>
-      <c r="M18" s="49"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
       <c r="N18" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="O18" s="49"/>
+      <c r="O18" s="47"/>
     </row>
     <row r="19" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
@@ -411,10 +1987,10 @@
         <v>194</v>
       </c>
       <c r="C19" s="14"/>
-      <c r="F19" s="40" t="s">
+      <c r="F19" s="38" t="s">
         <v>253</v>
       </c>
-      <c r="G19" s="42" t="s">
+      <c r="G19" s="40" t="s">
         <v>250</v>
       </c>
       <c r="I19" s="17"/>
@@ -468,10 +2044,10 @@
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="1"/>
-      <c r="F22" s="52" t="s">
+      <c r="F22" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="54"/>
+      <c r="G22" s="52"/>
       <c r="H22" s="1"/>
       <c r="I22" s="20"/>
       <c r="J22" s="20"/>
@@ -534,14 +2110,14 @@
       <c r="G25" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="I25" s="52" t="s">
+      <c r="I25" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="J25" s="53"/>
-      <c r="K25" s="53"/>
-      <c r="L25" s="53"/>
-      <c r="M25" s="53"/>
-      <c r="N25" s="54"/>
+      <c r="J25" s="55"/>
+      <c r="K25" s="55"/>
+      <c r="L25" s="55"/>
+      <c r="M25" s="55"/>
+      <c r="N25" s="52"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
     </row>
@@ -595,7 +2171,7 @@
       <c r="K27" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="L27" s="46" t="s">
+      <c r="L27" s="44" t="s">
         <v>256</v>
       </c>
       <c r="M27" s="14"/>
@@ -647,7 +2223,7 @@
       </c>
       <c r="L29" s="14"/>
       <c r="M29" s="14"/>
-      <c r="N29" s="27" t="s">
+      <c r="N29" s="25" t="s">
         <v>242</v>
       </c>
       <c r="R29" s="1"/>
@@ -659,10 +2235,10 @@
         <v>225</v>
       </c>
       <c r="C30" s="14"/>
-      <c r="F30" s="45" t="s">
+      <c r="F30" s="43" t="s">
         <v>258</v>
       </c>
-      <c r="G30" s="40" t="s">
+      <c r="G30" s="38" t="s">
         <v>251</v>
       </c>
       <c r="I30" s="14" t="s">
@@ -715,10 +2291,10 @@
       <c r="C33" s="17"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="52" t="s">
+      <c r="F33" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="G33" s="54"/>
+      <c r="G33" s="52"/>
       <c r="H33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
@@ -731,7 +2307,7 @@
       <c r="B34" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="C34" s="40" t="s">
+      <c r="C34" s="38" t="s">
         <v>269</v>
       </c>
       <c r="D34" s="1"/>
@@ -762,7 +2338,7 @@
       <c r="F35" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="G35" s="28"/>
+      <c r="G35" s="26"/>
       <c r="H35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
@@ -773,10 +2349,10 @@
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
-      <c r="B36" s="52" t="s">
+      <c r="B36" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="54"/>
+      <c r="C36" s="52"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="14" t="s">
@@ -784,15 +2360,15 @@
       </c>
       <c r="G36" s="10"/>
       <c r="H36" s="1"/>
-      <c r="I36" s="57" t="s">
+      <c r="I36" s="58" t="s">
         <v>244</v>
       </c>
-      <c r="J36" s="30" t="s">
+      <c r="J36" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="K36" s="31"/>
-      <c r="L36" s="31"/>
-      <c r="M36" s="32"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="30"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
@@ -815,15 +2391,15 @@
       </c>
       <c r="G37" s="10"/>
       <c r="H37" s="1"/>
-      <c r="I37" s="58"/>
-      <c r="J37" s="33" t="s">
+      <c r="I37" s="59"/>
+      <c r="J37" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="K37" s="59" t="s">
+      <c r="K37" s="53" t="s">
         <v>145</v>
       </c>
-      <c r="L37" s="59"/>
-      <c r="M37" s="60"/>
+      <c r="L37" s="53"/>
+      <c r="M37" s="54"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
@@ -846,11 +2422,11 @@
       </c>
       <c r="G38" s="10"/>
       <c r="H38" s="1"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="27"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
@@ -893,14 +2469,14 @@
         <v>227</v>
       </c>
       <c r="G40" s="10"/>
-      <c r="I40" s="52" t="s">
+      <c r="I40" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="J40" s="53"/>
-      <c r="K40" s="53"/>
-      <c r="L40" s="53"/>
-      <c r="M40" s="53"/>
-      <c r="N40" s="54"/>
+      <c r="J40" s="55"/>
+      <c r="K40" s="55"/>
+      <c r="L40" s="55"/>
+      <c r="M40" s="55"/>
+      <c r="N40" s="52"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
@@ -918,17 +2494,17 @@
       <c r="I41" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="J41" s="37" t="s">
+      <c r="J41" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="K41" s="38">
+      <c r="K41" s="36">
         <v>0.3</v>
       </c>
-      <c r="L41" s="67" t="s">
+      <c r="L41" s="66" t="s">
         <v>121</v>
       </c>
-      <c r="M41" s="67"/>
-      <c r="N41" s="50"/>
+      <c r="M41" s="66"/>
+      <c r="N41" s="48"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
@@ -939,10 +2515,10 @@
       <c r="A42" s="1"/>
       <c r="B42" s="9"/>
       <c r="C42" s="14"/>
-      <c r="F42" s="40" t="s">
+      <c r="F42" s="38" t="s">
         <v>248</v>
       </c>
-      <c r="G42" s="42" t="s">
+      <c r="G42" s="40" t="s">
         <v>280</v>
       </c>
       <c r="I42" s="14" t="s">
@@ -951,14 +2527,14 @@
       <c r="J42" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="K42" s="39">
+      <c r="K42" s="37">
         <v>0.3</v>
       </c>
-      <c r="L42" s="68" t="s">
+      <c r="L42" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="M42" s="68"/>
-      <c r="N42" s="51"/>
+      <c r="M42" s="67"/>
+      <c r="N42" s="49"/>
       <c r="O42" s="5"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
@@ -978,11 +2554,11 @@
       <c r="K43" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="L43" s="59" t="s">
+      <c r="L43" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="M43" s="59"/>
-      <c r="N43" s="60"/>
+      <c r="M43" s="53"/>
+      <c r="N43" s="54"/>
       <c r="O43" s="5"/>
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
@@ -994,7 +2570,7 @@
       <c r="B44" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="C44" s="40" t="s">
+      <c r="C44" s="38" t="s">
         <v>274</v>
       </c>
       <c r="O44" s="5"/>
@@ -1005,10 +2581,10 @@
     </row>
     <row r="45" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
-      <c r="F45" s="52" t="s">
+      <c r="F45" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="G45" s="54"/>
+      <c r="G45" s="52"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
@@ -1041,16 +2617,16 @@
       <c r="G47" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="I47" s="64" t="s">
+      <c r="I47" s="63" t="s">
         <v>45</v>
       </c>
       <c r="J47" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="K47" s="37" t="s">
+      <c r="K47" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="L47" s="28" t="s">
+      <c r="L47" s="26" t="s">
         <v>47</v>
       </c>
       <c r="M47" s="1"/>
@@ -1063,17 +2639,17 @@
     </row>
     <row r="48" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
-      <c r="B48" s="52" t="s">
+      <c r="B48" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="54"/>
+      <c r="C48" s="52"/>
       <c r="F48" s="14" t="s">
         <v>43</v>
       </c>
       <c r="G48" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I48" s="65"/>
+      <c r="I48" s="64"/>
       <c r="J48" s="9" t="s">
         <v>187</v>
       </c>
@@ -1099,7 +2675,7 @@
         <v>90</v>
       </c>
       <c r="G49" s="14"/>
-      <c r="I49" s="66"/>
+      <c r="I49" s="65"/>
       <c r="J49" s="11" t="s">
         <v>210</v>
       </c>
@@ -1126,7 +2702,7 @@
       <c r="F50" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="G50" s="43"/>
+      <c r="G50" s="41"/>
       <c r="H50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
@@ -1148,7 +2724,7 @@
       <c r="F51" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="G51" s="43" t="s">
+      <c r="G51" s="41" t="s">
         <v>289</v>
       </c>
       <c r="H51" s="1"/>
@@ -1174,7 +2750,7 @@
       <c r="F52" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="G52" s="40" t="s">
+      <c r="G52" s="38" t="s">
         <v>264</v>
       </c>
       <c r="H52" s="1"/>
@@ -1191,20 +2767,20 @@
     </row>
     <row r="53" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
-      <c r="B53" s="43" t="s">
+      <c r="B53" s="41" t="s">
         <v>249</v>
       </c>
       <c r="C53" s="14" t="s">
         <v>151</v>
       </c>
       <c r="H53" s="1"/>
-      <c r="I53" s="61" t="s">
+      <c r="I53" s="60" t="s">
         <v>245</v>
       </c>
       <c r="J53" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="K53" s="34">
+      <c r="K53" s="32">
         <v>0.5</v>
       </c>
       <c r="L53" s="1"/>
@@ -1220,18 +2796,18 @@
     </row>
     <row r="54" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
-      <c r="B54" s="40" t="s">
+      <c r="B54" s="38" t="s">
         <v>268</v>
       </c>
       <c r="C54" s="15" t="s">
         <v>197</v>
       </c>
       <c r="H54" s="1"/>
-      <c r="I54" s="62"/>
+      <c r="I54" s="61"/>
       <c r="J54" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="K54" s="35">
+      <c r="K54" s="33">
         <v>0.5</v>
       </c>
       <c r="M54" s="1"/>
@@ -1246,16 +2822,16 @@
     </row>
     <row r="55" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
-      <c r="F55" s="52" t="s">
+      <c r="F55" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="G55" s="54"/>
+      <c r="G55" s="52"/>
       <c r="H55" s="1"/>
-      <c r="I55" s="62"/>
+      <c r="I55" s="61"/>
       <c r="J55" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="K55" s="35">
+      <c r="K55" s="33">
         <v>0.5</v>
       </c>
     </row>
@@ -1268,20 +2844,20 @@
         <v>19</v>
       </c>
       <c r="H56" s="1"/>
-      <c r="I56" s="62"/>
+      <c r="I56" s="61"/>
       <c r="J56" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="K56" s="27" t="s">
+      <c r="K56" s="25" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="57" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
-      <c r="B57" s="52" t="s">
+      <c r="B57" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="C57" s="54"/>
+      <c r="C57" s="52"/>
       <c r="F57" s="16" t="s">
         <v>26</v>
       </c>
@@ -1289,11 +2865,11 @@
         <v>193</v>
       </c>
       <c r="H57" s="1"/>
-      <c r="I57" s="63"/>
+      <c r="I57" s="62"/>
       <c r="J57" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="K57" s="36" t="s">
+      <c r="K57" s="34" t="s">
         <v>224</v>
       </c>
       <c r="L57" s="7"/>
@@ -1326,7 +2902,7 @@
       <c r="C59" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="F59" s="43" t="s">
+      <c r="F59" s="41" t="s">
         <v>262</v>
       </c>
       <c r="G59" s="14" t="s">
@@ -1352,17 +2928,17 @@
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
-      <c r="F60" s="43" t="s">
+      <c r="F60" s="41" t="s">
         <v>286</v>
       </c>
       <c r="G60" s="14" t="s">
         <v>83</v>
       </c>
       <c r="H60" s="1"/>
-      <c r="I60" s="55" t="s">
+      <c r="I60" s="56" t="s">
         <v>243</v>
       </c>
-      <c r="J60" s="28" t="s">
+      <c r="J60" s="26" t="s">
         <v>44</v>
       </c>
       <c r="K60" s="1"/>
@@ -1385,13 +2961,13 @@
       <c r="C61" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="F61" s="40" t="s">
+      <c r="F61" s="38" t="s">
         <v>247</v>
       </c>
       <c r="G61" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="I61" s="56"/>
+      <c r="I61" s="57"/>
       <c r="J61" s="12" t="s">
         <v>74</v>
       </c>
@@ -1440,10 +3016,10 @@
         <v>167</v>
       </c>
       <c r="C63" s="14"/>
-      <c r="F63" s="52" t="s">
+      <c r="F63" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="G63" s="54"/>
+      <c r="G63" s="52"/>
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
@@ -1502,10 +3078,10 @@
         <v>178</v>
       </c>
       <c r="C65" s="14"/>
-      <c r="F65" s="46" t="s">
+      <c r="F65" s="44" t="s">
         <v>235</v>
       </c>
-      <c r="G65" s="46" t="s">
+      <c r="G65" s="44" t="s">
         <v>234</v>
       </c>
       <c r="M65" s="1"/>
@@ -1533,8 +3109,8 @@
       <c r="A66" s="1"/>
       <c r="B66" s="14"/>
       <c r="C66" s="14"/>
-      <c r="F66" s="47"/>
-      <c r="G66" s="43" t="s">
+      <c r="F66" s="45"/>
+      <c r="G66" s="41" t="s">
         <v>278</v>
       </c>
       <c r="M66" s="1"/>
@@ -1562,8 +3138,8 @@
       <c r="A67" s="1"/>
       <c r="B67" s="14"/>
       <c r="C67" s="14"/>
-      <c r="F67" s="47"/>
-      <c r="G67" s="43" t="s">
+      <c r="F67" s="45"/>
+      <c r="G67" s="41" t="s">
         <v>276</v>
       </c>
       <c r="M67" s="1"/>
@@ -1594,7 +3170,7 @@
       </c>
       <c r="C68" s="14"/>
       <c r="F68" s="17"/>
-      <c r="G68" s="43" t="s">
+      <c r="G68" s="41" t="s">
         <v>275</v>
       </c>
       <c r="M68" s="1"/>
@@ -1627,7 +3203,7 @@
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="17"/>
-      <c r="G69" s="43" t="s">
+      <c r="G69" s="41" t="s">
         <v>279</v>
       </c>
       <c r="H69" s="1"/>
@@ -1659,7 +3235,7 @@
       </c>
       <c r="C70" s="14"/>
       <c r="F70" s="15"/>
-      <c r="G70" s="40" t="s">
+      <c r="G70" s="38" t="s">
         <v>272</v>
       </c>
       <c r="H70" s="1"/>
@@ -1726,10 +3302,10 @@
         <v>129</v>
       </c>
       <c r="C73" s="14"/>
-      <c r="F73" s="52" t="s">
+      <c r="F73" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="G73" s="54"/>
+      <c r="G73" s="52"/>
       <c r="H73" s="1"/>
     </row>
     <row r="74" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1795,7 +3371,7 @@
         <v>59</v>
       </c>
       <c r="C79" s="14"/>
-      <c r="F79" s="40" t="s">
+      <c r="F79" s="38" t="s">
         <v>271</v>
       </c>
       <c r="G79" s="15" t="s">
@@ -1819,10 +3395,10 @@
         <v>172</v>
       </c>
       <c r="C82" s="14"/>
-      <c r="F82" s="52" t="s">
+      <c r="F82" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="G82" s="54"/>
+      <c r="G82" s="52"/>
     </row>
     <row r="83" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B83" s="14" t="s">
@@ -1849,7 +3425,9 @@
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B85" s="14"/>
+      <c r="B85" s="14" t="s">
+        <v>228</v>
+      </c>
       <c r="C85" s="14"/>
       <c r="F85" s="14"/>
       <c r="G85" s="14" t="s">
@@ -1857,7 +3435,9 @@
       </c>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B86" s="14"/>
+      <c r="B86" s="14" t="s">
+        <v>94</v>
+      </c>
       <c r="C86" s="14"/>
       <c r="F86" s="14"/>
       <c r="G86" s="14" t="s">
@@ -1866,51 +3446,51 @@
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87" s="14" t="s">
-        <v>228</v>
+        <v>62</v>
       </c>
       <c r="C87" s="14"/>
-      <c r="F87" s="43" t="s">
+      <c r="F87" s="41" t="s">
         <v>287</v>
       </c>
       <c r="G87" s="14"/>
     </row>
     <row r="88" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B88" s="14" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="C88" s="14"/>
-      <c r="F88" s="40" t="s">
+      <c r="F88" s="38" t="s">
         <v>259</v>
       </c>
-      <c r="G88" s="40" t="s">
+      <c r="G88" s="38" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" s="14" t="s">
-        <v>62</v>
+        <v>148</v>
       </c>
       <c r="C89" s="14"/>
     </row>
     <row r="90" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="14" t="s">
-        <v>64</v>
+        <v>176</v>
       </c>
       <c r="C90" s="14"/>
     </row>
     <row r="91" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B91" s="14" t="s">
-        <v>148</v>
+        <v>65</v>
       </c>
       <c r="C91" s="14"/>
-      <c r="F91" s="52" t="s">
+      <c r="F91" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="G91" s="54"/>
+      <c r="G91" s="52"/>
     </row>
     <row r="92" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B92" s="14" t="s">
-        <v>176</v>
+        <v>66</v>
       </c>
       <c r="C92" s="14"/>
       <c r="F92" s="21" t="s">
@@ -1922,19 +3502,19 @@
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B93" s="14" t="s">
-        <v>65</v>
+        <v>157</v>
       </c>
       <c r="C93" s="14"/>
       <c r="F93" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="G93" s="28" t="s">
+      <c r="G93" s="26" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94" s="14" t="s">
-        <v>66</v>
+        <v>147</v>
       </c>
       <c r="C94" s="14"/>
       <c r="F94" s="14" t="s">
@@ -1946,10 +3526,10 @@
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95" s="14" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="C95" s="14"/>
-      <c r="F95" s="47" t="s">
+      <c r="F95" s="45" t="s">
         <v>255</v>
       </c>
       <c r="G95" s="10" t="s">
@@ -1957,38 +3537,33 @@
       </c>
     </row>
     <row r="96" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="14" t="s">
-        <v>147</v>
-      </c>
+      <c r="B96" s="14"/>
       <c r="C96" s="14"/>
       <c r="F96" s="18"/>
-      <c r="G96" s="69" t="s">
+      <c r="G96" s="50" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B97" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="C97" s="14"/>
-    </row>
-    <row r="98" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="14"/>
-      <c r="C98" s="14"/>
-    </row>
+    <row r="97" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B97" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="C97" s="38" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="99" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="C99" s="40" t="s">
-        <v>263</v>
-      </c>
-      <c r="F99" s="52" t="s">
+      <c r="F99" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="G99" s="54"/>
+      <c r="G99" s="52"/>
     </row>
     <row r="100" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B100" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" s="52"/>
       <c r="F100" s="21" t="s">
         <v>18</v>
       </c>
@@ -1996,82 +3571,92 @@
         <v>19</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B101" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C101" s="21" t="s">
+        <v>19</v>
+      </c>
       <c r="F101" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="G101" s="28" t="s">
+      <c r="G101" s="26" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B102" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="C102" s="16" t="s">
+        <v>232</v>
+      </c>
       <c r="F102" s="14"/>
       <c r="G102" s="10" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="103" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B103" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C103" s="14" t="s">
+        <v>171</v>
+      </c>
       <c r="F103" s="14"/>
       <c r="G103" s="10" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="104" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="C104" s="54"/>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B104" s="9"/>
+      <c r="C104" s="14" t="s">
+        <v>199</v>
+      </c>
       <c r="F104" s="14"/>
       <c r="G104" s="10"/>
     </row>
     <row r="105" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C105" s="21" t="s">
-        <v>19</v>
+      <c r="B105" s="9"/>
+      <c r="C105" s="14" t="s">
+        <v>86</v>
       </c>
       <c r="F105" s="15"/>
-      <c r="G105" s="42" t="s">
+      <c r="G105" s="40" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B106" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="C106" s="16" t="s">
-        <v>232</v>
+      <c r="B106" s="9"/>
+      <c r="C106" s="45" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B107" s="9" t="s">
-        <v>154</v>
-      </c>
+      <c r="B107" s="9"/>
       <c r="C107" s="14" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="108" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B108" s="9"/>
       <c r="C108" s="14" t="s">
-        <v>171</v>
+        <v>81</v>
       </c>
     </row>
     <row r="109" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B109" s="9"/>
-      <c r="C109" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="F109" s="52" t="s">
+      <c r="C109" s="17"/>
+      <c r="F109" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="G109" s="54"/>
+      <c r="G109" s="52"/>
     </row>
     <row r="110" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B110" s="9"/>
-      <c r="C110" s="14" t="s">
-        <v>86</v>
+      <c r="C110" s="46" t="s">
+        <v>80</v>
       </c>
       <c r="F110" s="8" t="s">
         <v>18</v>
@@ -2080,98 +3665,76 @@
         <v>19</v>
       </c>
     </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B111" s="9"/>
-      <c r="C111" s="14" t="s">
-        <v>82</v>
+    <row r="111" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B111" s="43" t="s">
+        <v>288</v>
+      </c>
+      <c r="C111" s="38" t="s">
+        <v>254</v>
       </c>
       <c r="F111" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="G111" s="46" t="s">
+      <c r="G111" s="44" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="112" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B112" s="9"/>
-      <c r="C112" s="14" t="s">
-        <v>81</v>
-      </c>
       <c r="F112" s="14" t="s">
         <v>70</v>
       </c>
       <c r="G112" s="14"/>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B113" s="9"/>
-      <c r="C113" s="43"/>
+    <row r="113" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F113" s="14" t="s">
         <v>208</v>
       </c>
       <c r="G113" s="14"/>
     </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B114" s="9"/>
-      <c r="C114" s="43"/>
+    <row r="114" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F114" s="14" t="s">
         <v>168</v>
       </c>
       <c r="G114" s="14"/>
     </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B115" s="9"/>
-      <c r="C115" s="43" t="s">
-        <v>254</v>
-      </c>
+    <row r="115" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F115" s="14" t="s">
         <v>214</v>
       </c>
       <c r="G115" s="14"/>
     </row>
-    <row r="116" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="45" t="s">
-        <v>288</v>
-      </c>
-      <c r="C116" s="40" t="s">
-        <v>252</v>
-      </c>
+    <row r="116" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
     </row>
-    <row r="117" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F117" s="40" t="s">
+    <row r="117" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F117" s="38" t="s">
         <v>257</v>
       </c>
-      <c r="G117" s="40" t="s">
+      <c r="G117" s="38" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B119" s="25"/>
-      <c r="C119" s="25"/>
-    </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B120" s="26"/>
-      <c r="C120" s="26"/>
-    </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B121" s="20"/>
-      <c r="C121" s="20"/>
-    </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B122" s="20"/>
-      <c r="C122" s="20"/>
-    </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B123" s="20"/>
-      <c r="C123" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="I25:N25"/>
+    <mergeCell ref="I60:I61"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="I53:I57"/>
+    <mergeCell ref="I47:I49"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="I40:N40"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="L42:M42"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="L43:N43"/>
     <mergeCell ref="I2:O2"/>
-    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B100:C100"/>
     <mergeCell ref="F109:G109"/>
     <mergeCell ref="F99:G99"/>
     <mergeCell ref="F91:G91"/>
@@ -2184,20 +3747,6 @@
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="I15:O15"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="I25:N25"/>
-    <mergeCell ref="I60:I61"/>
-    <mergeCell ref="I36:I37"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="K37:M37"/>
-    <mergeCell ref="I53:I57"/>
-    <mergeCell ref="I47:I49"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="I40:N40"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="L42:M42"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B36:C36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Tinieblas por infortunio y Kinético por alud
</commit_message>
<xml_diff>
--- a/Movimientos.xlsx
+++ b/Movimientos.xlsx
@@ -419,9 +419,6 @@
     <t>Furia (20) - 100</t>
   </si>
   <si>
-    <t>Tinieblas (-) - 100</t>
-  </si>
-  <si>
     <t>Evasión</t>
   </si>
   <si>
@@ -893,20 +890,23 @@
     <t>Acua cola (90) - 90</t>
   </si>
   <si>
-    <t>Tajo aéreo (75) - 95</t>
-  </si>
-  <si>
     <t>Golpe aéreo (60) - 100</t>
   </si>
   <si>
     <t xml:space="preserve">Trueno (120) - 70 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tajo aéreo (75) - 95 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tinieblas (-) - 100 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -962,6 +962,20 @@
     <font>
       <sz val="9"/>
       <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1156,7 +1170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1297,6 +1311,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1579,8 +1596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E106" sqref="E106"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,7 +1660,7 @@
     </row>
     <row r="3" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C3" s="10"/>
       <c r="F3" s="19" t="s">
@@ -1668,15 +1685,15 @@
         <v>40</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O3" s="21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C4" s="10"/>
       <c r="F4" s="9" t="s">
@@ -1689,7 +1706,7 @@
         <v>127</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K4" s="16" t="s">
         <v>128</v>
@@ -1698,35 +1715,35 @@
         <v>96</v>
       </c>
       <c r="M4" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N4" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="O4" s="42"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C5" s="10"/>
       <c r="F5" s="9"/>
       <c r="G5" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K5" s="14"/>
       <c r="L5" s="14"/>
       <c r="M5" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N5" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O5" s="14"/>
     </row>
@@ -1741,7 +1758,7 @@
         <v>41</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
@@ -1758,7 +1775,7 @@
       </c>
       <c r="I7" s="14"/>
       <c r="J7" s="46" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
@@ -1768,14 +1785,14 @@
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B8" s="41" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C8" s="10"/>
       <c r="F8" s="9"/>
       <c r="G8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
@@ -1789,41 +1806,41 @@
       <c r="F9" s="9"/>
       <c r="G9" s="14"/>
       <c r="I9" s="41" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
       <c r="O9" s="41" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="38" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="17"/>
       <c r="I10" s="38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J10" s="38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K10" s="15"/>
       <c r="L10" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="M10" s="38" t="s">
         <v>281</v>
-      </c>
-      <c r="M10" s="38" t="s">
-        <v>282</v>
       </c>
       <c r="N10" s="38"/>
       <c r="O10" s="38"/>
@@ -1839,10 +1856,10 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="F11" s="43" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G11" s="38" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I11" s="20"/>
       <c r="J11" s="24"/>
@@ -1909,7 +1926,7 @@
         <v>115</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I16" s="21" t="s">
         <v>36</v>
@@ -1930,7 +1947,7 @@
         <v>55</v>
       </c>
       <c r="O16" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -1938,7 +1955,7 @@
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="F17" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G17" s="10"/>
       <c r="I17" s="16" t="s">
@@ -1956,7 +1973,7 @@
         <v>57</v>
       </c>
       <c r="O17" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -1966,51 +1983,51 @@
       <c r="F18" s="14"/>
       <c r="G18" s="10"/>
       <c r="I18" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J18" s="14" t="s">
         <v>71</v>
       </c>
       <c r="K18" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L18" s="47"/>
       <c r="M18" s="47"/>
       <c r="N18" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O18" s="47"/>
     </row>
     <row r="19" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C19" s="14"/>
       <c r="F19" s="38" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G19" s="40" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I19" s="17"/>
       <c r="J19" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L19" s="14"/>
       <c r="M19" s="14"/>
       <c r="N19" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O19" s="17"/>
     </row>
     <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C20" s="14"/>
       <c r="I20" s="18"/>
@@ -2018,8 +2035,8 @@
       <c r="K20" s="18"/>
       <c r="L20" s="15"/>
       <c r="M20" s="15"/>
-      <c r="N20" s="15" t="s">
-        <v>161</v>
+      <c r="N20" s="69" t="s">
+        <v>160</v>
       </c>
       <c r="O20" s="15"/>
     </row>
@@ -2095,7 +2112,7 @@
       <c r="C24" s="14"/>
       <c r="F24" s="19"/>
       <c r="G24" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
@@ -2103,7 +2120,7 @@
     <row r="25" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C25" s="14"/>
       <c r="F25" s="9"/>
@@ -2141,13 +2158,13 @@
         <v>105</v>
       </c>
       <c r="L26" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="M26" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="M26" s="23" t="s">
+      <c r="N26" s="8" t="s">
         <v>238</v>
-      </c>
-      <c r="N26" s="8" t="s">
-        <v>239</v>
       </c>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
@@ -2155,7 +2172,7 @@
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C27" s="14"/>
       <c r="F27" s="9"/>
@@ -2172,11 +2189,11 @@
         <v>106</v>
       </c>
       <c r="L27" s="44" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M27" s="14"/>
       <c r="N27" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
@@ -2187,21 +2204,21 @@
       <c r="C28" s="14"/>
       <c r="F28" s="9"/>
       <c r="G28" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I28" s="14" t="s">
         <v>126</v>
       </c>
       <c r="J28" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K28" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L28" s="14"/>
       <c r="M28" s="14"/>
       <c r="N28" s="14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
@@ -2224,7 +2241,7 @@
       <c r="L29" s="14"/>
       <c r="M29" s="14"/>
       <c r="N29" s="25" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
@@ -2232,17 +2249,17 @@
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C30" s="14"/>
       <c r="F30" s="43" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G30" s="38" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J30" s="14"/>
       <c r="K30" s="14"/>
@@ -2261,7 +2278,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="I31" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J31" s="18"/>
       <c r="K31" s="18"/>
@@ -2286,7 +2303,7 @@
     <row r="33" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C33" s="17"/>
       <c r="D33" s="1"/>
@@ -2305,10 +2322,10 @@
     <row r="34" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C34" s="38" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -2336,7 +2353,7 @@
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G35" s="26"/>
       <c r="H35" s="1"/>
@@ -2356,15 +2373,15 @@
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G36" s="10"/>
       <c r="H36" s="1"/>
       <c r="I36" s="58" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J36" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K36" s="29"/>
       <c r="L36" s="29"/>
@@ -2393,10 +2410,10 @@
       <c r="H37" s="1"/>
       <c r="I37" s="59"/>
       <c r="J37" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="K37" s="53" t="s">
         <v>144</v>
-      </c>
-      <c r="K37" s="53" t="s">
-        <v>145</v>
       </c>
       <c r="L37" s="53"/>
       <c r="M37" s="54"/>
@@ -2410,15 +2427,15 @@
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G38" s="10"/>
       <c r="H38" s="1"/>
@@ -2437,13 +2454,13 @@
     <row r="39" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C39" s="14"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G39" s="10"/>
       <c r="H39" s="1"/>
@@ -2466,7 +2483,7 @@
       </c>
       <c r="C40" s="14"/>
       <c r="F40" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G40" s="10"/>
       <c r="I40" s="51" t="s">
@@ -2516,10 +2533,10 @@
       <c r="B42" s="9"/>
       <c r="C42" s="14"/>
       <c r="F42" s="38" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G42" s="40" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I42" s="14" t="s">
         <v>61</v>
@@ -2568,10 +2585,10 @@
     <row r="44" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C44" s="38" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="O44" s="5"/>
       <c r="P44" s="1"/>
@@ -2646,12 +2663,12 @@
       <c r="F48" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G48" s="14" t="s">
-        <v>34</v>
+      <c r="G48" s="45" t="s">
+        <v>290</v>
       </c>
       <c r="I48" s="64"/>
       <c r="J48" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K48" s="20"/>
       <c r="L48" s="10"/>
@@ -2677,7 +2694,7 @@
       <c r="G49" s="14"/>
       <c r="I49" s="65"/>
       <c r="J49" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K49" s="22"/>
       <c r="L49" s="12"/>
@@ -2695,12 +2712,12 @@
         <v>68</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G50" s="41"/>
       <c r="H50" s="1"/>
@@ -2722,10 +2739,10 @@
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="G51" s="41" t="s">
-        <v>289</v>
+        <v>168</v>
+      </c>
+      <c r="G51" s="68" t="s">
+        <v>34</v>
       </c>
       <c r="H51" s="1"/>
       <c r="L51" s="1"/>
@@ -2747,11 +2764,11 @@
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
-      <c r="F52" s="15" t="s">
-        <v>290</v>
+      <c r="F52" s="38" t="s">
+        <v>288</v>
       </c>
       <c r="G52" s="38" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H52" s="1"/>
       <c r="L52" s="1"/>
@@ -2768,17 +2785,17 @@
     <row r="53" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="41" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="60" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J53" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K53" s="32">
         <v>0.5</v>
@@ -2797,15 +2814,15 @@
     <row r="54" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="38" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H54" s="1"/>
       <c r="I54" s="61"/>
       <c r="J54" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K54" s="33">
         <v>0.5</v>
@@ -2829,7 +2846,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="61"/>
       <c r="J55" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K55" s="33">
         <v>0.5</v>
@@ -2846,10 +2863,10 @@
       <c r="H56" s="1"/>
       <c r="I56" s="61"/>
       <c r="J56" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K56" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="57" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2858,19 +2875,19 @@
         <v>10</v>
       </c>
       <c r="C57" s="52"/>
-      <c r="F57" s="16" t="s">
-        <v>26</v>
+      <c r="F57" s="70" t="s">
+        <v>285</v>
       </c>
       <c r="G57" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H57" s="1"/>
       <c r="I57" s="62"/>
       <c r="J57" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="K57" s="34" t="s">
         <v>223</v>
-      </c>
-      <c r="K57" s="34" t="s">
-        <v>224</v>
       </c>
       <c r="L57" s="7"/>
     </row>
@@ -2882,9 +2899,11 @@
       <c r="C58" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F58" s="14"/>
+      <c r="F58" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="G58" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H58" s="1"/>
       <c r="K58" s="6"/>
@@ -2902,9 +2921,7 @@
       <c r="C59" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="F59" s="41" t="s">
-        <v>262</v>
-      </c>
+      <c r="F59" s="41"/>
       <c r="G59" s="14" t="s">
         <v>87</v>
       </c>
@@ -2921,22 +2938,22 @@
     <row r="60" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="41" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
       <c r="G60" s="14" t="s">
         <v>83</v>
       </c>
       <c r="H60" s="1"/>
       <c r="I60" s="56" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J60" s="26" t="s">
         <v>44</v>
@@ -2959,10 +2976,10 @@
         <v>20</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F61" s="38" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G61" s="15" t="s">
         <v>84</v>
@@ -3013,7 +3030,7 @@
     <row r="63" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C63" s="14"/>
       <c r="F63" s="51" t="s">
@@ -3075,14 +3092,14 @@
     <row r="65" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C65" s="14"/>
       <c r="F65" s="44" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G65" s="44" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
@@ -3111,7 +3128,7 @@
       <c r="C66" s="14"/>
       <c r="F66" s="45"/>
       <c r="G66" s="41" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="M66" s="1"/>
       <c r="N66" s="1"/>
@@ -3140,7 +3157,7 @@
       <c r="C67" s="14"/>
       <c r="F67" s="45"/>
       <c r="G67" s="41" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="M67" s="1"/>
       <c r="N67" s="1"/>
@@ -3171,7 +3188,7 @@
       <c r="C68" s="14"/>
       <c r="F68" s="17"/>
       <c r="G68" s="41" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
@@ -3197,14 +3214,14 @@
     <row r="69" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C69" s="14"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="17"/>
       <c r="G69" s="41" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H69" s="1"/>
       <c r="M69" s="1"/>
@@ -3236,7 +3253,7 @@
       <c r="C70" s="14"/>
       <c r="F70" s="15"/>
       <c r="G70" s="38" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H70" s="1"/>
       <c r="M70" s="5"/>
@@ -3323,11 +3340,11 @@
     </row>
     <row r="75" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B75" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C75" s="14"/>
       <c r="F75" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G75" s="16" t="s">
         <v>111</v>
@@ -3336,7 +3353,7 @@
     </row>
     <row r="76" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B76" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C76" s="14"/>
       <c r="F76" s="14" t="s">
@@ -3363,7 +3380,7 @@
       <c r="C78" s="14"/>
       <c r="F78" s="14"/>
       <c r="G78" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="79" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3372,15 +3389,15 @@
       </c>
       <c r="C79" s="14"/>
       <c r="F79" s="38" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G79" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="80" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B80" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C80" s="14"/>
     </row>
@@ -3392,7 +3409,7 @@
     </row>
     <row r="82" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C82" s="14"/>
       <c r="F82" s="51" t="s">
@@ -3414,24 +3431,24 @@
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C84" s="14"/>
       <c r="F84" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="G84" s="16" t="s">
-        <v>131</v>
+        <v>148</v>
+      </c>
+      <c r="G84" s="44" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C85" s="14"/>
       <c r="F85" s="14"/>
       <c r="G85" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.25">
@@ -3441,7 +3458,7 @@
       <c r="C86" s="14"/>
       <c r="F86" s="14"/>
       <c r="G86" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.25">
@@ -3450,7 +3467,7 @@
       </c>
       <c r="C87" s="14"/>
       <c r="F87" s="41" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G87" s="14"/>
     </row>
@@ -3460,21 +3477,21 @@
       </c>
       <c r="C88" s="14"/>
       <c r="F88" s="38" t="s">
-        <v>259</v>
-      </c>
-      <c r="G88" s="38" t="s">
-        <v>267</v>
+        <v>258</v>
+      </c>
+      <c r="G88" s="69" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C89" s="14"/>
     </row>
     <row r="90" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C90" s="14"/>
     </row>
@@ -3502,11 +3519,11 @@
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B93" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C93" s="14"/>
       <c r="F93" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G93" s="26" t="s">
         <v>112</v>
@@ -3514,7 +3531,7 @@
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C94" s="14"/>
       <c r="F94" s="14" t="s">
@@ -3526,14 +3543,14 @@
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C95" s="14"/>
       <c r="F95" s="45" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G95" s="10" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="96" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3541,15 +3558,15 @@
       <c r="C96" s="14"/>
       <c r="F96" s="18"/>
       <c r="G96" s="50" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="97" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B97" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C97" s="38" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="98" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3579,7 +3596,7 @@
         <v>19</v>
       </c>
       <c r="F101" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G101" s="26" t="s">
         <v>110</v>
@@ -3587,32 +3604,32 @@
     </row>
     <row r="102" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B102" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C102" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F102" s="14"/>
       <c r="G102" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B103" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F103" s="14"/>
       <c r="G103" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B104" s="9"/>
       <c r="C104" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F104" s="14"/>
       <c r="G104" s="10"/>
@@ -3624,13 +3641,13 @@
       </c>
       <c r="F105" s="15"/>
       <c r="G105" s="40" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106" s="9"/>
       <c r="C106" s="45" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
@@ -3667,16 +3684,16 @@
     </row>
     <row r="111" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B111" s="43" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C111" s="38" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F111" s="16" t="s">
         <v>69</v>
       </c>
       <c r="G111" s="44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="112" spans="2:7" x14ac:dyDescent="0.25">
@@ -3687,19 +3704,19 @@
     </row>
     <row r="113" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F113" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G113" s="14"/>
     </row>
     <row r="114" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F114" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G114" s="14"/>
     </row>
     <row r="115" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F115" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G115" s="14"/>
     </row>
@@ -3709,10 +3726,10 @@
     </row>
     <row r="117" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F117" s="38" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G117" s="38" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ataque furia por foco resplandor
</commit_message>
<xml_diff>
--- a/Movimientos.xlsx
+++ b/Movimientos.xlsx
@@ -1596,8 +1596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="I110" sqref="I110"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2110,9 +2110,9 @@
         <v>56</v>
       </c>
       <c r="C24" s="14"/>
-      <c r="F24" s="19"/>
+      <c r="F24" s="16"/>
       <c r="G24" s="16" t="s">
-        <v>173</v>
+        <v>124</v>
       </c>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
@@ -2123,9 +2123,9 @@
         <v>220</v>
       </c>
       <c r="C25" s="14"/>
-      <c r="F25" s="9"/>
+      <c r="F25" s="14"/>
       <c r="G25" s="14" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="I25" s="51" t="s">
         <v>100</v>
@@ -2144,9 +2144,9 @@
         <v>91</v>
       </c>
       <c r="C26" s="14"/>
-      <c r="F26" s="9"/>
+      <c r="F26" s="14"/>
       <c r="G26" s="14" t="s">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="I26" s="23" t="s">
         <v>101</v>
@@ -2175,9 +2175,9 @@
         <v>212</v>
       </c>
       <c r="C27" s="14"/>
-      <c r="F27" s="9"/>
+      <c r="F27" s="14"/>
       <c r="G27" s="14" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
       <c r="I27" s="16" t="s">
         <v>102</v>
@@ -2202,10 +2202,8 @@
       <c r="A28" s="1"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="14" t="s">
-        <v>164</v>
-      </c>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
       <c r="I28" s="14" t="s">
         <v>126</v>
       </c>
@@ -2227,8 +2225,10 @@
       <c r="A29" s="1"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="46" t="s">
+        <v>173</v>
+      </c>
       <c r="I29" s="14" t="s">
         <v>107</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>224</v>
       </c>
       <c r="C30" s="14"/>
-      <c r="F30" s="43" t="s">
+      <c r="F30" s="38" t="s">
         <v>257</v>
       </c>
       <c r="G30" s="38" t="s">

</xml_diff>

<commit_message>
cabezazo zen por refugio
</commit_message>
<xml_diff>
--- a/Movimientos.xlsx
+++ b/Movimientos.xlsx
@@ -1601,7 +1601,7 @@
   <dimension ref="A1:AF117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1738,7 +1738,7 @@
         <v>203</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>180</v>
+        <v>41</v>
       </c>
       <c r="J5" s="14" t="s">
         <v>139</v>
@@ -1762,9 +1762,7 @@
       <c r="G6" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="I6" s="14" t="s">
-        <v>41</v>
-      </c>
+      <c r="I6" s="14"/>
       <c r="J6" s="14" t="s">
         <v>140</v>
       </c>
@@ -1798,7 +1796,9 @@
       <c r="C8" s="40"/>
       <c r="F8" s="9"/>
       <c r="G8" s="17"/>
-      <c r="I8" s="14"/>
+      <c r="I8" s="46" t="s">
+        <v>180</v>
+      </c>
       <c r="J8" s="14" t="s">
         <v>174</v>
       </c>

</xml_diff>

<commit_message>
Explosión por tijera X
</commit_message>
<xml_diff>
--- a/Movimientos.xlsx
+++ b/Movimientos.xlsx
@@ -251,9 +251,6 @@
     <t>(18) - 85</t>
   </si>
   <si>
-    <t>Bomba sónica (20 ps)</t>
-  </si>
-  <si>
     <t>Ácido (40) - 100)</t>
   </si>
   <si>
@@ -287,9 +284,6 @@
     <t>Rayo aurora (65) - 100</t>
   </si>
   <si>
-    <t>Hiperrayo (150) - 90</t>
-  </si>
-  <si>
     <t>Picotazo (35)</t>
   </si>
   <si>
@@ -900,6 +894,12 @@
   </si>
   <si>
     <t xml:space="preserve">Malicioso (1 nivel) - 100 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bomba sónica (20 ps) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiperrayo (150) - 90  </t>
   </si>
 </sst>
 </file>
@@ -1614,8 +1614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="K81" sqref="K81"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,16 +1669,16 @@
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>68</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
@@ -1686,40 +1686,40 @@
         <v>27</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F4" s="56" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="18"/>
       <c r="C6" s="50" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F6" s="57"/>
       <c r="G6" s="14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F7" s="43" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G7" s="18"/>
     </row>
@@ -1759,16 +1759,16 @@
     </row>
     <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C11" s="58" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F11" s="19" t="s">
         <v>49</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I11" s="21" t="s">
         <v>36</v>
@@ -1786,80 +1786,80 @@
         <v>40</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="O11" s="21" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C12" s="10"/>
       <c r="F12" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="G12" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="G12" s="14" t="s">
-        <v>98</v>
-      </c>
       <c r="I12" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J12" s="59" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M12" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="N12" s="16" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="O12" s="42"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="45" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C13" s="10"/>
       <c r="F13" s="9"/>
       <c r="G13" s="14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I13" s="14" t="s">
         <v>41</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
       <c r="M13" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="N13" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="O13" s="14"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C14" s="10"/>
       <c r="F14" s="9"/>
       <c r="G14" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I14" s="14"/>
       <c r="J14" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
@@ -1872,11 +1872,11 @@
       <c r="C15" s="10"/>
       <c r="F15" s="9"/>
       <c r="G15" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I15" s="14"/>
       <c r="J15" s="53" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
@@ -1886,16 +1886,16 @@
     </row>
     <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="38" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C16" s="40"/>
       <c r="F16" s="9"/>
       <c r="G16" s="17"/>
       <c r="I16" s="46" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J16" s="46" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
@@ -1905,39 +1905,39 @@
     </row>
     <row r="17" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F17" s="43" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G17" s="38" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="I17" s="41" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J17" s="46" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
       <c r="M17" s="14"/>
       <c r="N17" s="14"/>
       <c r="O17" s="41" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="I18" s="38" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J18" s="38" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="K18" s="15"/>
       <c r="L18" s="38" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="M18" s="38" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="N18" s="38"/>
       <c r="O18" s="38"/>
@@ -1987,7 +1987,7 @@
     <row r="22" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C22" s="14"/>
       <c r="F22" s="60" t="s">
@@ -1998,7 +1998,7 @@
     <row r="23" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="14" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C23" s="14"/>
       <c r="F23" s="21" t="s">
@@ -2024,10 +2024,10 @@
       </c>
       <c r="C24" s="14"/>
       <c r="F24" s="16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G24" s="26" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I24" s="21" t="s">
         <v>36</v>
@@ -2048,27 +2048,27 @@
         <v>55</v>
       </c>
       <c r="O24" s="21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C25" s="14"/>
       <c r="F25" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G25" s="10"/>
       <c r="I25" s="16" t="s">
         <v>72</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="K25" s="16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L25" s="21"/>
       <c r="M25" s="21"/>
@@ -2076,7 +2076,7 @@
         <v>57</v>
       </c>
       <c r="O25" s="16" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
@@ -2086,22 +2086,22 @@
       </c>
       <c r="C26" s="14"/>
       <c r="F26" s="45" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G26" s="10"/>
       <c r="I26" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K26" s="14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L26" s="47"/>
       <c r="M26" s="47"/>
       <c r="N26" s="14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="O26" s="47"/>
     </row>
@@ -2113,24 +2113,24 @@
       <c r="C27" s="14"/>
       <c r="F27" s="38"/>
       <c r="G27" s="40" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I27" s="17"/>
       <c r="J27" s="14"/>
       <c r="K27" s="14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="L27" s="14"/>
       <c r="M27" s="14"/>
       <c r="N27" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="O27" s="17"/>
     </row>
     <row r="28" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C28" s="14"/>
       <c r="I28" s="18"/>
@@ -2141,14 +2141,14 @@
       <c r="L28" s="15"/>
       <c r="M28" s="15"/>
       <c r="N28" s="54" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O28" s="15"/>
     </row>
     <row r="29" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C29" s="14"/>
       <c r="I29" s="20"/>
@@ -2162,7 +2162,7 @@
     <row r="30" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C30" s="14"/>
       <c r="D30" s="1"/>
@@ -2186,7 +2186,7 @@
     <row r="31" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="14" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C31" s="14"/>
       <c r="D31" s="1"/>
@@ -2216,10 +2216,10 @@
       </c>
       <c r="C32" s="17"/>
       <c r="F32" s="44" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
@@ -2232,10 +2232,10 @@
       <c r="C33" s="17"/>
       <c r="F33" s="14"/>
       <c r="G33" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I33" s="60" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J33" s="62"/>
       <c r="K33" s="62"/>
@@ -2248,30 +2248,30 @@
     <row r="34" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C34" s="17"/>
       <c r="F34" s="14"/>
       <c r="G34" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I34" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="J34" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="J34" s="23" t="s">
+      <c r="K34" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="K34" s="23" t="s">
-        <v>104</v>
-      </c>
       <c r="L34" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="M34" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="N34" s="8" t="s">
         <v>234</v>
-      </c>
-      <c r="M34" s="23" t="s">
-        <v>235</v>
-      </c>
-      <c r="N34" s="8" t="s">
-        <v>236</v>
       </c>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
@@ -2279,30 +2279,30 @@
     <row r="35" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F35" s="14"/>
       <c r="G35" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I35" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="J35" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="J35" s="16" t="s">
+      <c r="K35" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="K35" s="16" t="s">
-        <v>105</v>
-      </c>
       <c r="L35" s="44" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="M35" s="14"/>
       <c r="N35" s="16" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
@@ -2312,18 +2312,18 @@
       <c r="F36" s="17"/>
       <c r="G36" s="17"/>
       <c r="I36" s="14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J36" s="14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K36" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="L36" s="14"/>
       <c r="M36" s="14"/>
       <c r="N36" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
@@ -2332,21 +2332,21 @@
       <c r="A37" s="1"/>
       <c r="F37" s="14"/>
       <c r="G37" s="46" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J37" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K37" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L37" s="14"/>
       <c r="M37" s="14"/>
       <c r="N37" s="25" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
@@ -2359,10 +2359,10 @@
       <c r="C38" s="61"/>
       <c r="F38" s="38"/>
       <c r="G38" s="38" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J38" s="14"/>
       <c r="K38" s="14"/>
@@ -2383,7 +2383,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="I39" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J39" s="18"/>
       <c r="K39" s="18"/>
@@ -2396,10 +2396,10 @@
     <row r="40" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -2410,10 +2410,10 @@
     <row r="41" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C41" s="45" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -2431,7 +2431,7 @@
     <row r="42" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C42" s="14"/>
       <c r="D42" s="1"/>
@@ -2458,13 +2458,13 @@
     <row r="43" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C43" s="14"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G43" s="26"/>
       <c r="H43" s="1"/>
@@ -2482,15 +2482,15 @@
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="14" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G44" s="10"/>
       <c r="H44" s="1"/>
       <c r="I44" s="65" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="J44" s="28" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K44" s="29"/>
       <c r="L44" s="29"/>
@@ -2505,7 +2505,7 @@
     <row r="45" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C45" s="38"/>
       <c r="D45" s="1"/>
@@ -2517,10 +2517,10 @@
       <c r="H45" s="1"/>
       <c r="I45" s="66"/>
       <c r="J45" s="31" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K45" s="67" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L45" s="67"/>
       <c r="M45" s="68"/>
@@ -2536,7 +2536,7 @@
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G46" s="10"/>
       <c r="H46" s="1"/>
@@ -2557,7 +2557,7 @@
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G47" s="10"/>
       <c r="H47" s="1"/>
@@ -2580,7 +2580,7 @@
       </c>
       <c r="C48" s="61"/>
       <c r="F48" s="14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G48" s="10"/>
       <c r="I48" s="60" t="s">
@@ -2617,7 +2617,7 @@
         <v>0.3</v>
       </c>
       <c r="L49" s="75" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M49" s="75"/>
       <c r="N49" s="48"/>
@@ -2630,16 +2630,16 @@
     <row r="50" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="19" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F50" s="38" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G50" s="40" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="I50" s="14" t="s">
         <v>61</v>
@@ -2651,7 +2651,7 @@
         <v>0.3</v>
       </c>
       <c r="L50" s="76" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M50" s="76"/>
       <c r="N50" s="49"/>
@@ -2664,22 +2664,22 @@
     <row r="51" spans="1:21" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I51" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="J51" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="K51" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="J51" s="22" t="s">
+      <c r="L51" s="67" t="s">
         <v>117</v>
-      </c>
-      <c r="K51" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="L51" s="67" t="s">
-        <v>119</v>
       </c>
       <c r="M51" s="67"/>
       <c r="N51" s="68"/>
@@ -2693,7 +2693,7 @@
       <c r="A52" s="1"/>
       <c r="B52" s="9"/>
       <c r="C52" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="O52" s="5"/>
       <c r="P52" s="1"/>
@@ -2705,7 +2705,7 @@
       <c r="A53" s="1"/>
       <c r="B53" s="9"/>
       <c r="C53" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F53" s="60" t="s">
         <v>17</v>
@@ -2723,7 +2723,7 @@
       <c r="A54" s="1"/>
       <c r="B54" s="9"/>
       <c r="C54" s="45" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>18</v>
@@ -2743,10 +2743,10 @@
       <c r="A55" s="1"/>
       <c r="B55" s="9"/>
       <c r="C55" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F55" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G55" s="16" t="s">
         <v>42</v>
@@ -2775,17 +2775,17 @@
       <c r="A56" s="1"/>
       <c r="B56" s="9"/>
       <c r="C56" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F56" s="14" t="s">
         <v>43</v>
       </c>
       <c r="G56" s="45" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="I56" s="73"/>
       <c r="J56" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K56" s="20"/>
       <c r="L56" s="10"/>
@@ -2802,12 +2802,12 @@
       <c r="B57" s="9"/>
       <c r="C57" s="17"/>
       <c r="F57" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G57" s="14"/>
       <c r="I57" s="74"/>
       <c r="J57" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K57" s="22"/>
       <c r="L57" s="12"/>
@@ -2823,12 +2823,12 @@
       <c r="A58" s="1"/>
       <c r="B58" s="9"/>
       <c r="C58" s="46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G58" s="41"/>
       <c r="H58" s="1"/>
@@ -2846,15 +2846,15 @@
     <row r="59" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="43" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C59" s="38" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G59" s="52" t="s">
         <v>34</v>
@@ -2876,10 +2876,10 @@
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="38" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G60" s="38" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H60" s="1"/>
       <c r="L60" s="1"/>
@@ -2897,10 +2897,10 @@
       <c r="A61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="69" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J61" s="16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K61" s="32">
         <v>0.5</v>
@@ -2925,7 +2925,7 @@
       <c r="H62" s="1"/>
       <c r="I62" s="70"/>
       <c r="J62" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K62" s="33">
         <v>0.5</v>
@@ -2955,7 +2955,7 @@
       <c r="H63" s="1"/>
       <c r="I63" s="70"/>
       <c r="J63" s="14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K63" s="33">
         <v>0.5</v>
@@ -2964,10 +2964,10 @@
     <row r="64" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="F64" s="8" t="s">
         <v>18</v>
@@ -2978,10 +2978,10 @@
       <c r="H64" s="1"/>
       <c r="I64" s="70"/>
       <c r="J64" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="K64" s="25" t="s">
         <v>219</v>
-      </c>
-      <c r="K64" s="25" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="65" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2990,37 +2990,37 @@
         <v>20</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="F65" s="55" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G65" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="71"/>
       <c r="J65" s="15" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="K65" s="34" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="L65" s="7"/>
     </row>
     <row r="66" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="C66" s="14" t="s">
-        <v>179</v>
+        <v>162</v>
+      </c>
+      <c r="C66" s="45" t="s">
+        <v>258</v>
       </c>
       <c r="F66" s="14" t="s">
         <v>26</v>
       </c>
       <c r="G66" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H66" s="1"/>
       <c r="K66" s="6"/>
@@ -3036,11 +3036,11 @@
         <v>63</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>87</v>
+        <v>291</v>
       </c>
       <c r="F67" s="41"/>
       <c r="G67" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
@@ -3055,20 +3055,20 @@
     <row r="68" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C68" s="14"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="41" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G68" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H68" s="1"/>
       <c r="I68" s="63" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J68" s="26" t="s">
         <v>44</v>
@@ -3088,14 +3088,14 @@
     <row r="69" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C69" s="14"/>
       <c r="F69" s="38" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G69" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I69" s="64"/>
       <c r="J69" s="12" t="s">
@@ -3116,7 +3116,7 @@
     <row r="70" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C70" s="14"/>
       <c r="M70" s="1"/>
@@ -3197,7 +3197,7 @@
     <row r="73" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C73" s="14"/>
       <c r="F73" s="8" t="s">
@@ -3236,10 +3236,10 @@
       </c>
       <c r="C74" s="14"/>
       <c r="F74" s="44" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G74" s="44" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I74" s="78"/>
       <c r="J74" s="78"/>
@@ -3267,12 +3267,12 @@
     <row r="75" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C75" s="14"/>
       <c r="F75" s="45"/>
       <c r="G75" s="45" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I75" s="79"/>
       <c r="J75" s="79"/>
@@ -3300,12 +3300,12 @@
     <row r="76" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C76" s="14"/>
       <c r="F76" s="45"/>
       <c r="G76" s="41" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I76" s="79"/>
       <c r="J76" s="80"/>
@@ -3340,7 +3340,7 @@
       <c r="E77" s="1"/>
       <c r="F77" s="17"/>
       <c r="G77" s="41" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H77" s="1"/>
       <c r="I77" s="79"/>
@@ -3374,7 +3374,7 @@
       <c r="C78" s="14"/>
       <c r="F78" s="17"/>
       <c r="G78" s="41" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="24"/>
@@ -3407,7 +3407,7 @@
       <c r="C79" s="14"/>
       <c r="F79" s="15"/>
       <c r="G79" s="38" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="24"/>
@@ -3435,7 +3435,7 @@
     </row>
     <row r="80" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C80" s="14"/>
       <c r="G80" s="2"/>
@@ -3456,7 +3456,7 @@
     </row>
     <row r="82" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C82" s="14"/>
       <c r="F82" s="8" t="s">
@@ -3473,43 +3473,43 @@
       </c>
       <c r="C83" s="14"/>
       <c r="F83" s="16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G83" s="16" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H83" s="1"/>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C84" s="14"/>
       <c r="F84" s="14" t="s">
         <v>25</v>
       </c>
       <c r="G84" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" s="14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C85" s="14"/>
       <c r="F85" s="14"/>
       <c r="G85" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B86" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C86" s="14"/>
       <c r="F86" s="14"/>
       <c r="G86" s="14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="87" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3518,10 +3518,10 @@
       </c>
       <c r="C87" s="14"/>
       <c r="F87" s="38" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G87" s="15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
@@ -3532,13 +3532,13 @@
     </row>
     <row r="89" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B89" s="14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C89" s="14"/>
     </row>
     <row r="90" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C90" s="14"/>
       <c r="F90" s="60" t="s">
@@ -3564,39 +3564,39 @@
       </c>
       <c r="C92" s="14"/>
       <c r="F92" s="16" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G92" s="44" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C93" s="14"/>
       <c r="F93" s="14"/>
       <c r="G93" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C94" s="14"/>
       <c r="F94" s="14"/>
       <c r="G94" s="14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B95" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C95" s="14"/>
       <c r="F95" s="41" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G95" s="14"/>
     </row>
@@ -3604,15 +3604,15 @@
       <c r="B96" s="17"/>
       <c r="C96" s="14"/>
       <c r="F96" s="38" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G96" s="54" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B97" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C97" s="14"/>
     </row>
@@ -3624,7 +3624,7 @@
     </row>
     <row r="99" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B99" s="52" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C99" s="17"/>
       <c r="F99" s="60" t="s">
@@ -3636,8 +3636,8 @@
       <c r="B100" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="C100" s="38" t="s">
-        <v>260</v>
+      <c r="C100" s="51" t="s">
+        <v>290</v>
       </c>
       <c r="F100" s="21" t="s">
         <v>18</v>
@@ -3648,16 +3648,16 @@
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F101" s="16" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G101" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="102" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F102" s="14"/>
       <c r="G102" s="10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="103" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3667,7 +3667,7 @@
       <c r="C103" s="61"/>
       <c r="F103" s="14"/>
       <c r="G103" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="104" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3685,11 +3685,11 @@
         <v>69</v>
       </c>
       <c r="C105" s="44" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F105" s="15"/>
       <c r="G105" s="40" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.25">
@@ -3697,24 +3697,24 @@
         <v>70</v>
       </c>
       <c r="C106" s="45" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B107" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C107" s="14"/>
     </row>
     <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B108" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C108" s="14"/>
     </row>
     <row r="109" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B109" s="14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C109" s="14"/>
     </row>
@@ -3724,7 +3724,7 @@
     </row>
     <row r="111" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B111" s="38" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C111" s="38"/>
     </row>

</xml_diff>

<commit_message>
Casa del hombre ocupado en ruta 30
</commit_message>
<xml_diff>
--- a/Movimientos.xlsx
+++ b/Movimientos.xlsx
@@ -509,9 +509,6 @@
     <t>Comesueños (100) - 100</t>
   </si>
   <si>
-    <t>Gas venenoso (90)</t>
-  </si>
-  <si>
     <t>Bombardeo (15x2a5) - 85</t>
   </si>
   <si>
@@ -900,6 +897,9 @@
   </si>
   <si>
     <t xml:space="preserve">Hiperrayo (150) - 90  </t>
+  </si>
+  <si>
+    <t>Gas venenoso (75)</t>
   </si>
 </sst>
 </file>
@@ -1176,7 +1176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1275,26 +1275,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1320,18 +1311,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1614,8 +1616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1644,14 +1646,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="F1" s="60" t="s">
+      <c r="C1" s="65"/>
+      <c r="F1" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="61"/>
+      <c r="G1" s="65"/>
     </row>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="21" t="s">
@@ -1669,7 +1671,7 @@
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>109</v>
@@ -1689,7 +1691,7 @@
         <v>110</v>
       </c>
       <c r="F4" s="56" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>75</v>
@@ -1697,10 +1699,10 @@
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="14" t="s">
@@ -1710,29 +1712,29 @@
     <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="18"/>
       <c r="C6" s="50" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F6" s="57"/>
       <c r="G6" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F7" s="43" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="61"/>
-      <c r="F9" s="60" t="s">
+      <c r="C9" s="65"/>
+      <c r="F9" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="61"/>
+      <c r="G9" s="65"/>
     </row>
     <row r="10" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
@@ -1747,22 +1749,22 @@
       <c r="G10" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="60" t="s">
+      <c r="I10" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="62"/>
-      <c r="O10" s="61"/>
+      <c r="J10" s="74"/>
+      <c r="K10" s="74"/>
+      <c r="L10" s="74"/>
+      <c r="M10" s="74"/>
+      <c r="N10" s="74"/>
+      <c r="O10" s="65"/>
     </row>
     <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C11" s="58" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F11" s="19" t="s">
         <v>49</v>
@@ -1789,12 +1791,12 @@
         <v>128</v>
       </c>
       <c r="O11" s="21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C12" s="10"/>
       <c r="F12" s="9" t="s">
@@ -1807,7 +1809,7 @@
         <v>124</v>
       </c>
       <c r="J12" s="59" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K12" s="16" t="s">
         <v>125</v>
@@ -1819,18 +1821,18 @@
         <v>155</v>
       </c>
       <c r="N12" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="O12" s="42"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="45" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C13" s="10"/>
       <c r="F13" s="9"/>
       <c r="G13" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I13" s="14" t="s">
         <v>41</v>
@@ -1850,7 +1852,7 @@
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C14" s="10"/>
       <c r="F14" s="9"/>
@@ -1859,7 +1861,7 @@
       </c>
       <c r="I14" s="14"/>
       <c r="J14" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
@@ -1886,16 +1888,16 @@
     </row>
     <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="38" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C16" s="40"/>
       <c r="F16" s="9"/>
       <c r="G16" s="17"/>
       <c r="I16" s="46" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J16" s="46" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
@@ -1905,13 +1907,13 @@
     </row>
     <row r="17" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F17" s="43" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G17" s="38" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I17" s="41" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J17" s="46" t="s">
         <v>135</v>
@@ -1921,23 +1923,23 @@
       <c r="M17" s="14"/>
       <c r="N17" s="14"/>
       <c r="O17" s="41" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="I18" s="38" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J18" s="38" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K18" s="15"/>
       <c r="L18" s="38" t="s">
+        <v>275</v>
+      </c>
+      <c r="M18" s="38" t="s">
         <v>276</v>
-      </c>
-      <c r="M18" s="38" t="s">
-        <v>277</v>
       </c>
       <c r="N18" s="38"/>
       <c r="O18" s="38"/>
@@ -1951,10 +1953,10 @@
     </row>
     <row r="19" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="61"/>
+      <c r="C19" s="65"/>
       <c r="I19" s="20"/>
       <c r="J19" s="24"/>
       <c r="K19" s="20"/>
@@ -1987,18 +1989,18 @@
     <row r="22" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C22" s="14"/>
-      <c r="F22" s="60" t="s">
+      <c r="F22" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="61"/>
+      <c r="G22" s="65"/>
     </row>
     <row r="23" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C23" s="14"/>
       <c r="F23" s="21" t="s">
@@ -2007,15 +2009,15 @@
       <c r="G23" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="60" t="s">
+      <c r="I23" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="J23" s="62"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="62"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="62"/>
-      <c r="O23" s="61"/>
+      <c r="J23" s="74"/>
+      <c r="K23" s="74"/>
+      <c r="L23" s="74"/>
+      <c r="M23" s="74"/>
+      <c r="N23" s="74"/>
+      <c r="O23" s="65"/>
     </row>
     <row r="24" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
@@ -2027,7 +2029,7 @@
         <v>112</v>
       </c>
       <c r="G24" s="26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I24" s="21" t="s">
         <v>36</v>
@@ -2058,14 +2060,14 @@
       </c>
       <c r="C25" s="14"/>
       <c r="F25" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G25" s="10"/>
       <c r="I25" s="16" t="s">
         <v>72</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K25" s="16" t="s">
         <v>106</v>
@@ -2076,7 +2078,7 @@
         <v>57</v>
       </c>
       <c r="O25" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
@@ -2086,17 +2088,17 @@
       </c>
       <c r="C26" s="14"/>
       <c r="F26" s="45" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G26" s="10"/>
       <c r="I26" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J26" s="14" t="s">
         <v>132</v>
       </c>
       <c r="K26" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L26" s="47"/>
       <c r="M26" s="47"/>
@@ -2113,12 +2115,12 @@
       <c r="C27" s="14"/>
       <c r="F27" s="38"/>
       <c r="G27" s="40" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I27" s="17"/>
       <c r="J27" s="14"/>
       <c r="K27" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L27" s="14"/>
       <c r="M27" s="14"/>
@@ -2130,7 +2132,7 @@
     <row r="28" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C28" s="14"/>
       <c r="I28" s="18"/>
@@ -2162,14 +2164,14 @@
     <row r="30" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C30" s="14"/>
       <c r="D30" s="1"/>
-      <c r="F30" s="60" t="s">
+      <c r="F30" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="G30" s="61"/>
+      <c r="G30" s="65"/>
       <c r="H30" s="1"/>
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
@@ -2186,7 +2188,7 @@
     <row r="31" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C31" s="14"/>
       <c r="D31" s="1"/>
@@ -2216,7 +2218,7 @@
       </c>
       <c r="C32" s="17"/>
       <c r="F32" s="44" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G32" s="16" t="s">
         <v>121</v>
@@ -2234,14 +2236,14 @@
       <c r="G33" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="I33" s="60" t="s">
+      <c r="I33" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="J33" s="62"/>
-      <c r="K33" s="62"/>
-      <c r="L33" s="62"/>
-      <c r="M33" s="62"/>
-      <c r="N33" s="61"/>
+      <c r="J33" s="74"/>
+      <c r="K33" s="74"/>
+      <c r="L33" s="74"/>
+      <c r="M33" s="74"/>
+      <c r="N33" s="65"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
     </row>
@@ -2265,13 +2267,13 @@
         <v>102</v>
       </c>
       <c r="L34" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="M34" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="M34" s="23" t="s">
+      <c r="N34" s="8" t="s">
         <v>233</v>
-      </c>
-      <c r="N34" s="8" t="s">
-        <v>234</v>
       </c>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
@@ -2279,10 +2281,10 @@
     <row r="35" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F35" s="14"/>
       <c r="G35" s="14" t="s">
@@ -2298,11 +2300,11 @@
         <v>103</v>
       </c>
       <c r="L35" s="44" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M35" s="14"/>
       <c r="N35" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
@@ -2315,7 +2317,7 @@
         <v>123</v>
       </c>
       <c r="J36" s="14" t="s">
-        <v>161</v>
+        <v>291</v>
       </c>
       <c r="K36" s="14" t="s">
         <v>159</v>
@@ -2323,7 +2325,7 @@
       <c r="L36" s="14"/>
       <c r="M36" s="14"/>
       <c r="N36" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
@@ -2332,7 +2334,7 @@
       <c r="A37" s="1"/>
       <c r="F37" s="14"/>
       <c r="G37" s="46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I37" s="14" t="s">
         <v>104</v>
@@ -2346,23 +2348,23 @@
       <c r="L37" s="14"/>
       <c r="M37" s="14"/>
       <c r="N37" s="25" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
-      <c r="B38" s="60" t="s">
+      <c r="B38" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="61"/>
+      <c r="C38" s="65"/>
       <c r="F38" s="38"/>
       <c r="G38" s="38" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J38" s="14"/>
       <c r="K38" s="14"/>
@@ -2383,7 +2385,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="I39" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J39" s="18"/>
       <c r="K39" s="18"/>
@@ -2396,10 +2398,10 @@
     <row r="40" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -2413,14 +2415,14 @@
         <v>147</v>
       </c>
       <c r="C41" s="45" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="60" t="s">
+      <c r="F41" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="G41" s="61"/>
+      <c r="G41" s="65"/>
       <c r="H41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
@@ -2464,7 +2466,7 @@
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G43" s="26"/>
       <c r="H43" s="1"/>
@@ -2482,12 +2484,12 @@
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G44" s="10"/>
       <c r="H44" s="1"/>
-      <c r="I44" s="65" t="s">
-        <v>239</v>
+      <c r="I44" s="79" t="s">
+        <v>238</v>
       </c>
       <c r="J44" s="28" t="s">
         <v>138</v>
@@ -2505,7 +2507,7 @@
     <row r="45" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C45" s="38"/>
       <c r="D45" s="1"/>
@@ -2515,15 +2517,15 @@
       </c>
       <c r="G45" s="10"/>
       <c r="H45" s="1"/>
-      <c r="I45" s="66"/>
+      <c r="I45" s="80"/>
       <c r="J45" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="K45" s="67" t="s">
+      <c r="K45" s="66" t="s">
         <v>140</v>
       </c>
-      <c r="L45" s="67"/>
-      <c r="M45" s="68"/>
+      <c r="L45" s="66"/>
+      <c r="M45" s="67"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
@@ -2536,7 +2538,7 @@
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G46" s="10"/>
       <c r="H46" s="1"/>
@@ -2557,7 +2559,7 @@
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G47" s="10"/>
       <c r="H47" s="1"/>
@@ -2575,22 +2577,22 @@
     </row>
     <row r="48" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
-      <c r="B48" s="60" t="s">
+      <c r="B48" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C48" s="61"/>
+      <c r="C48" s="65"/>
       <c r="F48" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G48" s="10"/>
-      <c r="I48" s="60" t="s">
+      <c r="I48" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="J48" s="62"/>
-      <c r="K48" s="62"/>
-      <c r="L48" s="62"/>
-      <c r="M48" s="62"/>
-      <c r="N48" s="61"/>
+      <c r="J48" s="74"/>
+      <c r="K48" s="74"/>
+      <c r="L48" s="74"/>
+      <c r="M48" s="74"/>
+      <c r="N48" s="65"/>
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
@@ -2633,13 +2635,13 @@
         <v>150</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F50" s="38" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G50" s="40" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I50" s="14" t="s">
         <v>61</v>
@@ -2667,7 +2669,7 @@
         <v>149</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I51" s="15" t="s">
         <v>114</v>
@@ -2678,11 +2680,11 @@
       <c r="K51" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="L51" s="67" t="s">
+      <c r="L51" s="66" t="s">
         <v>117</v>
       </c>
-      <c r="M51" s="67"/>
-      <c r="N51" s="68"/>
+      <c r="M51" s="66"/>
+      <c r="N51" s="67"/>
       <c r="O51" s="5"/>
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
@@ -2693,7 +2695,7 @@
       <c r="A52" s="1"/>
       <c r="B52" s="9"/>
       <c r="C52" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O52" s="5"/>
       <c r="P52" s="1"/>
@@ -2707,10 +2709,10 @@
       <c r="C53" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="F53" s="60" t="s">
+      <c r="F53" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="G53" s="61"/>
+      <c r="G53" s="65"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
@@ -2723,7 +2725,7 @@
       <c r="A54" s="1"/>
       <c r="B54" s="9"/>
       <c r="C54" s="45" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>18</v>
@@ -2751,7 +2753,7 @@
       <c r="G55" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="I55" s="72" t="s">
+      <c r="I55" s="71" t="s">
         <v>45</v>
       </c>
       <c r="J55" s="19" t="s">
@@ -2781,11 +2783,11 @@
         <v>43</v>
       </c>
       <c r="G56" s="45" t="s">
-        <v>286</v>
-      </c>
-      <c r="I56" s="73"/>
+        <v>285</v>
+      </c>
+      <c r="I56" s="72"/>
       <c r="J56" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K56" s="20"/>
       <c r="L56" s="10"/>
@@ -2805,9 +2807,9 @@
         <v>87</v>
       </c>
       <c r="G57" s="14"/>
-      <c r="I57" s="74"/>
+      <c r="I57" s="73"/>
       <c r="J57" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K57" s="22"/>
       <c r="L57" s="12"/>
@@ -2828,7 +2830,7 @@
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G58" s="41"/>
       <c r="H58" s="1"/>
@@ -2846,15 +2848,15 @@
     <row r="59" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="43" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C59" s="38" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G59" s="52" t="s">
         <v>34</v>
@@ -2876,10 +2878,10 @@
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G60" s="38" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H60" s="1"/>
       <c r="L60" s="1"/>
@@ -2896,8 +2898,8 @@
     <row r="61" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="H61" s="1"/>
-      <c r="I61" s="69" t="s">
-        <v>240</v>
+      <c r="I61" s="68" t="s">
+        <v>239</v>
       </c>
       <c r="J61" s="16" t="s">
         <v>129</v>
@@ -2918,12 +2920,12 @@
     </row>
     <row r="62" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
-      <c r="B62" s="60" t="s">
+      <c r="B62" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="C62" s="61"/>
+      <c r="C62" s="65"/>
       <c r="H62" s="1"/>
-      <c r="I62" s="70"/>
+      <c r="I62" s="69"/>
       <c r="J62" s="14" t="s">
         <v>157</v>
       </c>
@@ -2948,14 +2950,14 @@
       <c r="C63" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F63" s="60" t="s">
+      <c r="F63" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="G63" s="61"/>
+      <c r="G63" s="65"/>
       <c r="H63" s="1"/>
-      <c r="I63" s="70"/>
+      <c r="I63" s="69"/>
       <c r="J63" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K63" s="33">
         <v>0.5</v>
@@ -2966,7 +2968,7 @@
       <c r="B64" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C64" s="16" t="s">
+      <c r="C64" s="26" t="s">
         <v>151</v>
       </c>
       <c r="F64" s="8" t="s">
@@ -2976,12 +2978,12 @@
         <v>19</v>
       </c>
       <c r="H64" s="1"/>
-      <c r="I64" s="70"/>
+      <c r="I64" s="69"/>
       <c r="J64" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K64" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="65" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2989,38 +2991,38 @@
       <c r="B65" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C65" s="14" t="s">
-        <v>177</v>
+      <c r="C65" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="F65" s="55" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G65" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H65" s="1"/>
-      <c r="I65" s="71"/>
+      <c r="I65" s="70"/>
       <c r="J65" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="K65" s="34" t="s">
         <v>218</v>
-      </c>
-      <c r="K65" s="34" t="s">
-        <v>219</v>
       </c>
       <c r="L65" s="7"/>
     </row>
     <row r="66" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="C66" s="45" t="s">
-        <v>258</v>
+        <v>161</v>
+      </c>
+      <c r="C66" s="58" t="s">
+        <v>257</v>
       </c>
       <c r="F66" s="14" t="s">
         <v>26</v>
       </c>
       <c r="G66" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H66" s="1"/>
       <c r="K66" s="6"/>
@@ -3035,8 +3037,8 @@
       <c r="B67" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C67" s="14" t="s">
-        <v>291</v>
+      <c r="C67" s="10" t="s">
+        <v>290</v>
       </c>
       <c r="F67" s="41"/>
       <c r="G67" s="14" t="s">
@@ -3055,20 +3057,20 @@
     <row r="68" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="C68" s="14"/>
+        <v>172</v>
+      </c>
+      <c r="C68" s="10"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="41" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G68" s="14" t="s">
         <v>81</v>
       </c>
       <c r="H68" s="1"/>
-      <c r="I68" s="63" t="s">
-        <v>238</v>
+      <c r="I68" s="77" t="s">
+        <v>237</v>
       </c>
       <c r="J68" s="26" t="s">
         <v>44</v>
@@ -3090,14 +3092,14 @@
       <c r="B69" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="C69" s="14"/>
+      <c r="C69" s="10"/>
       <c r="F69" s="38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G69" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="I69" s="64"/>
+      <c r="I69" s="78"/>
       <c r="J69" s="12" t="s">
         <v>73</v>
       </c>
@@ -3118,7 +3120,7 @@
       <c r="B70" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="C70" s="14"/>
+      <c r="C70" s="10"/>
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
       <c r="O70" s="1"/>
@@ -3143,7 +3145,7 @@
       <c r="B71" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C71" s="14"/>
+      <c r="C71" s="10"/>
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
@@ -3168,11 +3170,11 @@
       <c r="B72" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C72" s="14"/>
-      <c r="F72" s="60" t="s">
+      <c r="C72" s="10"/>
+      <c r="F72" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="G72" s="61"/>
+      <c r="G72" s="65"/>
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
@@ -3199,15 +3201,15 @@
       <c r="B73" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="C73" s="14"/>
+      <c r="C73" s="10"/>
       <c r="F73" s="8" t="s">
         <v>18</v>
       </c>
       <c r="G73" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I73" s="77"/>
-      <c r="J73" s="77"/>
+      <c r="I73" s="60"/>
+      <c r="J73" s="60"/>
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
@@ -3234,15 +3236,15 @@
       <c r="B74" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C74" s="14"/>
+      <c r="C74" s="10"/>
       <c r="F74" s="44" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G74" s="44" t="s">
-        <v>270</v>
-      </c>
-      <c r="I74" s="78"/>
-      <c r="J74" s="78"/>
+        <v>269</v>
+      </c>
+      <c r="I74" s="61"/>
+      <c r="J74" s="61"/>
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
@@ -3267,15 +3269,15 @@
     <row r="75" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="C75" s="14"/>
+        <v>184</v>
+      </c>
+      <c r="C75" s="10"/>
       <c r="F75" s="45"/>
       <c r="G75" s="45" t="s">
-        <v>229</v>
-      </c>
-      <c r="I75" s="79"/>
-      <c r="J75" s="79"/>
+        <v>228</v>
+      </c>
+      <c r="I75" s="62"/>
+      <c r="J75" s="62"/>
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
@@ -3300,15 +3302,15 @@
     <row r="76" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="C76" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="C76" s="10"/>
       <c r="F76" s="45"/>
       <c r="G76" s="41" t="s">
-        <v>271</v>
-      </c>
-      <c r="I76" s="79"/>
-      <c r="J76" s="80"/>
+        <v>270</v>
+      </c>
+      <c r="I76" s="62"/>
+      <c r="J76" s="63"/>
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
       <c r="O76" s="1"/>
@@ -3335,16 +3337,16 @@
       <c r="B77" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C77" s="14"/>
+      <c r="C77" s="10"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="17"/>
       <c r="G77" s="41" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H77" s="1"/>
-      <c r="I77" s="79"/>
-      <c r="J77" s="80"/>
+      <c r="I77" s="62"/>
+      <c r="J77" s="63"/>
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
       <c r="O77" s="1"/>
@@ -3371,14 +3373,14 @@
       <c r="B78" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C78" s="14"/>
+      <c r="C78" s="10"/>
       <c r="F78" s="17"/>
       <c r="G78" s="41" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="24"/>
-      <c r="J78" s="80"/>
+      <c r="J78" s="63"/>
       <c r="M78" s="5"/>
       <c r="N78" s="1"/>
       <c r="O78" s="1"/>
@@ -3404,14 +3406,14 @@
       <c r="B79" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C79" s="14"/>
+      <c r="C79" s="10"/>
       <c r="F79" s="15"/>
       <c r="G79" s="38" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="24"/>
-      <c r="J79" s="80"/>
+      <c r="J79" s="63"/>
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
@@ -3435,30 +3437,30 @@
     </row>
     <row r="80" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="C80" s="14"/>
+        <v>178</v>
+      </c>
+      <c r="C80" s="10"/>
       <c r="G80" s="2"/>
       <c r="H80" s="1"/>
       <c r="I80" s="20"/>
-      <c r="J80" s="80"/>
+      <c r="J80" s="63"/>
     </row>
     <row r="81" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C81" s="14"/>
-      <c r="F81" s="60" t="s">
+      <c r="C81" s="10"/>
+      <c r="F81" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="G81" s="61"/>
+      <c r="G81" s="65"/>
       <c r="H81" s="1"/>
     </row>
     <row r="82" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="C82" s="14"/>
+        <v>166</v>
+      </c>
+      <c r="C82" s="10"/>
       <c r="F82" s="8" t="s">
         <v>18</v>
       </c>
@@ -3471,9 +3473,9 @@
       <c r="B83" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C83" s="14"/>
+      <c r="C83" s="10"/>
       <c r="F83" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G83" s="16" t="s">
         <v>108</v>
@@ -3482,9 +3484,9 @@
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="C84" s="14"/>
+        <v>174</v>
+      </c>
+      <c r="C84" s="10"/>
       <c r="F84" s="14" t="s">
         <v>25</v>
       </c>
@@ -3494,9 +3496,9 @@
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="C85" s="14"/>
+        <v>222</v>
+      </c>
+      <c r="C85" s="10"/>
       <c r="F85" s="14"/>
       <c r="G85" s="14" t="s">
         <v>77</v>
@@ -3506,19 +3508,19 @@
       <c r="B86" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C86" s="14"/>
+      <c r="C86" s="10"/>
       <c r="F86" s="14"/>
       <c r="G86" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="87" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B87" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C87" s="14"/>
+      <c r="C87" s="10"/>
       <c r="F87" s="38" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G87" s="15" t="s">
         <v>148</v>
@@ -3528,29 +3530,29 @@
       <c r="B88" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C88" s="14"/>
+      <c r="C88" s="10"/>
     </row>
     <row r="89" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B89" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="C89" s="14"/>
+      <c r="C89" s="10"/>
     </row>
     <row r="90" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="C90" s="14"/>
-      <c r="F90" s="60" t="s">
+        <v>170</v>
+      </c>
+      <c r="C90" s="10"/>
+      <c r="F90" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="G90" s="61"/>
+      <c r="G90" s="65"/>
     </row>
     <row r="91" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B91" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C91" s="14"/>
+      <c r="C91" s="10"/>
       <c r="F91" s="8" t="s">
         <v>18</v>
       </c>
@@ -3562,82 +3564,82 @@
       <c r="B92" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C92" s="14"/>
+      <c r="C92" s="10"/>
       <c r="F92" s="16" t="s">
         <v>144</v>
       </c>
       <c r="G92" s="44" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="C93" s="14"/>
+      <c r="C93" s="10"/>
       <c r="F93" s="14"/>
       <c r="G93" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="C94" s="14"/>
+      <c r="C94" s="10"/>
       <c r="F94" s="14"/>
       <c r="G94" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="C95" s="14"/>
+      <c r="B95" s="14"/>
+      <c r="C95" s="10"/>
       <c r="F95" s="41" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G95" s="14"/>
     </row>
     <row r="96" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="17"/>
-      <c r="C96" s="14"/>
+      <c r="B96" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="C96" s="10"/>
       <c r="F96" s="38" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G96" s="54" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B97" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="C97" s="14"/>
+      <c r="B97" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C97" s="10"/>
     </row>
     <row r="98" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="C98" s="14"/>
+      <c r="B98" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="C98" s="10"/>
     </row>
     <row r="99" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="52" t="s">
-        <v>154</v>
-      </c>
-      <c r="C99" s="17"/>
-      <c r="F99" s="60" t="s">
+      <c r="B99" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="C99" s="82"/>
+      <c r="F99" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="G99" s="61"/>
+      <c r="G99" s="65"/>
     </row>
     <row r="100" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B100" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="C100" s="51" t="s">
-        <v>290</v>
+        <v>171</v>
+      </c>
+      <c r="C100" s="50" t="s">
+        <v>289</v>
       </c>
       <c r="F100" s="21" t="s">
         <v>18</v>
@@ -3648,7 +3650,7 @@
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F101" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G101" s="26" t="s">
         <v>107</v>
@@ -3657,21 +3659,21 @@
     <row r="102" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F102" s="14"/>
       <c r="G102" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="103" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="60" t="s">
+      <c r="B103" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="C103" s="61"/>
+      <c r="C103" s="65"/>
       <c r="F103" s="14"/>
       <c r="G103" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="104" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="8" t="s">
+      <c r="B104" s="21" t="s">
         <v>18</v>
       </c>
       <c r="C104" s="8" t="s">
@@ -3684,52 +3686,68 @@
       <c r="B105" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C105" s="44" t="s">
+      <c r="C105" s="81" t="s">
         <v>130</v>
       </c>
       <c r="F105" s="15"/>
       <c r="G105" s="40" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C106" s="45" t="s">
-        <v>280</v>
+      <c r="C106" s="58" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B107" s="14" t="s">
-        <v>203</v>
-      </c>
-      <c r="C107" s="14"/>
+        <v>202</v>
+      </c>
+      <c r="C107" s="10"/>
     </row>
     <row r="108" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B108" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="C108" s="14"/>
+      <c r="B108" s="45" t="s">
+        <v>251</v>
+      </c>
+      <c r="C108" s="10"/>
     </row>
     <row r="109" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B109" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="C109" s="14"/>
+        <v>162</v>
+      </c>
+      <c r="C109" s="10"/>
     </row>
     <row r="110" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B110" s="14"/>
-      <c r="C110" s="14"/>
+      <c r="B110" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="C110" s="10"/>
     </row>
     <row r="111" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="38" t="s">
-        <v>252</v>
-      </c>
-      <c r="C111" s="38"/>
+      <c r="B111" s="18"/>
+      <c r="C111" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="I68:I69"/>
+    <mergeCell ref="I44:I45"/>
+    <mergeCell ref="I10:O10"/>
+    <mergeCell ref="I23:O23"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="I33:N33"/>
+    <mergeCell ref="K45:M45"/>
+    <mergeCell ref="I61:I65"/>
+    <mergeCell ref="I55:I57"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="I48:N48"/>
+    <mergeCell ref="L49:M49"/>
+    <mergeCell ref="L50:M50"/>
+    <mergeCell ref="L51:N51"/>
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="B103:C103"/>
     <mergeCell ref="F99:G99"/>
@@ -3743,23 +3761,7 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="F72:G72"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="K45:M45"/>
-    <mergeCell ref="I61:I65"/>
-    <mergeCell ref="I55:I57"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="I48:N48"/>
-    <mergeCell ref="L49:M49"/>
-    <mergeCell ref="L50:M50"/>
     <mergeCell ref="F9:G9"/>
-    <mergeCell ref="L51:N51"/>
-    <mergeCell ref="I10:O10"/>
-    <mergeCell ref="I23:O23"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="I33:N33"/>
-    <mergeCell ref="I68:I69"/>
-    <mergeCell ref="I44:I45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>